<commit_message>
Added door a key labels
</commit_message>
<xml_diff>
--- a/Assets/Documents/Game Document.xlsx
+++ b/Assets/Documents/Game Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\Horror_FPS\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C4A372-7F44-4AC4-A136-250B823053C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EAB796-C308-434D-AFD6-F31FB365DE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="9705" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nursery_big" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="235">
   <si>
     <t>Item</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Redondo</t>
   </si>
   <si>
-    <t>Triangulo</t>
-  </si>
-  <si>
     <t>Rojo</t>
   </si>
   <si>
@@ -715,6 +712,30 @@
   </si>
   <si>
     <t>Triángulo</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>Hexagon</t>
+  </si>
+  <si>
+    <t>Triangle</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Yellow</t>
   </si>
 </sst>
 </file>
@@ -745,7 +766,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,12 +854,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1197,7 +1212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1506,10 +1521,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2191,7 +2205,7 @@
       <c r="T9" s="10"/>
       <c r="U9" s="11"/>
       <c r="V9" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="W9" s="11"/>
       <c r="X9" s="12"/>
@@ -2201,7 +2215,7 @@
       <c r="AB9" s="12"/>
       <c r="AC9" s="11"/>
       <c r="AD9" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AE9" s="11"/>
       <c r="AF9" s="16"/>
@@ -2228,7 +2242,7 @@
       <c r="BA9" s="55"/>
       <c r="BB9" s="56"/>
       <c r="BC9" s="56" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BD9" s="56"/>
       <c r="BE9" s="63"/>
@@ -2360,7 +2374,7 @@
       <c r="AI11" s="53"/>
       <c r="AJ11" s="53"/>
       <c r="AK11" s="53" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AL11" s="53"/>
       <c r="AM11" s="53"/>
@@ -2372,7 +2386,7 @@
       <c r="AS11" s="53"/>
       <c r="AT11" s="53"/>
       <c r="AU11" s="53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AV11" s="53"/>
       <c r="AW11" s="53"/>
@@ -2532,7 +2546,7 @@
       <c r="BC13" s="59"/>
       <c r="BD13" s="59"/>
       <c r="BE13" s="59" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="BF13" s="59"/>
       <c r="BG13" s="59"/>
@@ -2573,7 +2587,7 @@
       <c r="T14" s="10"/>
       <c r="U14" s="11"/>
       <c r="V14" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="W14" s="11"/>
       <c r="X14" s="12"/>
@@ -2583,7 +2597,7 @@
       <c r="AB14" s="12"/>
       <c r="AC14" s="11"/>
       <c r="AD14" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AE14" s="11"/>
       <c r="AF14" s="16"/>
@@ -2968,7 +2982,7 @@
       <c r="Q19" s="84"/>
       <c r="R19" s="84"/>
       <c r="S19" s="84" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="T19" s="84"/>
       <c r="U19" s="84"/>
@@ -3361,7 +3375,7 @@
       <c r="S24" s="20"/>
       <c r="T24" s="21"/>
       <c r="U24" s="21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="V24" s="21"/>
       <c r="W24" s="21"/>
@@ -3371,7 +3385,7 @@
       <c r="AA24" s="92"/>
       <c r="AB24" s="21"/>
       <c r="AC24" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="AD24" s="21"/>
       <c r="AE24" s="21"/>
@@ -3529,7 +3543,7 @@
       <c r="AI26" s="53"/>
       <c r="AJ26" s="53"/>
       <c r="AK26" s="53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AL26" s="53"/>
       <c r="AM26" s="53"/>
@@ -3541,7 +3555,7 @@
       <c r="AS26" s="53"/>
       <c r="AT26" s="53"/>
       <c r="AU26" s="53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AV26" s="53"/>
       <c r="AW26" s="53"/>
@@ -3620,7 +3634,7 @@
       <c r="BC27" s="30"/>
       <c r="BD27" s="30"/>
       <c r="BE27" s="30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="BF27" s="30"/>
       <c r="BG27" s="30"/>
@@ -4590,8 +4604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A7:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4607,7 +4621,7 @@
   <sheetData>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -4633,10 +4647,10 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" t="s">
         <v>75</v>
-      </c>
-      <c r="B10" t="s">
-        <v>76</v>
       </c>
       <c r="C10" s="34" t="s">
         <v>1</v>
@@ -4656,18 +4670,18 @@
         <v>34</v>
       </c>
       <c r="L10" s="33" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M10" s="33" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11" t="s">
         <v>77</v>
-      </c>
-      <c r="B11" t="s">
-        <v>78</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>2</v>
@@ -4676,7 +4690,7 @@
       <c r="E11" s="33"/>
       <c r="F11" s="33"/>
       <c r="I11" s="33" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J11" s="34">
         <v>1</v>
@@ -4693,10 +4707,10 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
         <v>79</v>
-      </c>
-      <c r="B12" t="s">
-        <v>80</v>
       </c>
       <c r="C12" s="34" t="s">
         <v>3</v>
@@ -4705,7 +4719,7 @@
       <c r="E12" s="33"/>
       <c r="F12" s="33"/>
       <c r="I12" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" s="34">
         <v>2</v>
@@ -4722,10 +4736,10 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
         <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>82</v>
       </c>
       <c r="C13" s="34" t="s">
         <v>4</v>
@@ -4734,7 +4748,7 @@
       <c r="E13" s="33"/>
       <c r="F13" s="33"/>
       <c r="I13" s="33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13" s="34">
         <v>3</v>
@@ -4751,19 +4765,19 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C14" s="107" t="s">
+      <c r="C14" s="106" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="33"/>
       <c r="E14" s="33"/>
       <c r="F14" s="33"/>
       <c r="I14" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14" s="34">
         <v>4</v>
@@ -4780,10 +4794,10 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" t="s">
         <v>85</v>
-      </c>
-      <c r="B15" t="s">
-        <v>86</v>
       </c>
       <c r="C15" s="33"/>
       <c r="D15" s="33"/>
@@ -4792,10 +4806,10 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" t="s">
         <v>87</v>
-      </c>
-      <c r="B16" t="s">
-        <v>88</v>
       </c>
       <c r="C16" s="34" t="s">
         <v>6</v>
@@ -4806,10 +4820,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>88</v>
+      </c>
+      <c r="B17" t="s">
         <v>89</v>
-      </c>
-      <c r="B17" t="s">
-        <v>90</v>
       </c>
       <c r="C17" s="34" t="s">
         <v>7</v>
@@ -4824,10 +4838,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
         <v>91</v>
-      </c>
-      <c r="B18" t="s">
-        <v>92</v>
       </c>
       <c r="C18" s="34" t="s">
         <v>8</v>
@@ -4835,25 +4849,25 @@
       <c r="D18" s="33"/>
       <c r="E18" s="33"/>
       <c r="F18" s="33"/>
-      <c r="H18" s="106" t="s">
-        <v>47</v>
+      <c r="H18" s="108" t="s">
+        <v>46</v>
       </c>
       <c r="I18" s="34">
         <v>2</v>
       </c>
       <c r="J18" s="35" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
         <v>93</v>
-      </c>
-      <c r="B19" t="s">
-        <v>94</v>
       </c>
       <c r="C19" s="34" t="s">
         <v>9</v>
@@ -4861,25 +4875,25 @@
       <c r="D19" s="33"/>
       <c r="E19" s="33"/>
       <c r="F19" s="33"/>
-      <c r="H19" s="106" t="s">
-        <v>48</v>
+      <c r="H19" s="108" t="s">
+        <v>47</v>
       </c>
       <c r="I19" s="34">
         <v>13</v>
       </c>
       <c r="J19" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
         <v>95</v>
-      </c>
-      <c r="B20" t="s">
-        <v>96</v>
       </c>
       <c r="C20" s="34" t="s">
         <v>10</v>
@@ -4887,25 +4901,25 @@
       <c r="D20" s="33"/>
       <c r="E20" s="33"/>
       <c r="F20" s="33"/>
-      <c r="H20" s="106" t="s">
-        <v>49</v>
+      <c r="H20" s="108" t="s">
+        <v>48</v>
       </c>
       <c r="I20" s="34">
         <v>10</v>
       </c>
       <c r="J20" s="35" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
         <v>97</v>
-      </c>
-      <c r="B21" t="s">
-        <v>98</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>11</v>
@@ -4913,25 +4927,25 @@
       <c r="D21" s="33"/>
       <c r="E21" s="33"/>
       <c r="F21" s="33"/>
-      <c r="H21" s="106" t="s">
-        <v>50</v>
+      <c r="H21" s="108" t="s">
+        <v>49</v>
       </c>
       <c r="I21" s="34">
         <v>11</v>
       </c>
       <c r="J21" s="35" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="K21" s="35" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
         <v>99</v>
-      </c>
-      <c r="B22" t="s">
-        <v>100</v>
       </c>
       <c r="C22" s="34" t="s">
         <v>12</v>
@@ -4943,25 +4957,25 @@
         <v>20</v>
       </c>
       <c r="F22" s="33"/>
-      <c r="H22" s="106" t="s">
-        <v>51</v>
+      <c r="H22" s="108" t="s">
+        <v>50</v>
       </c>
       <c r="I22" s="34">
         <v>3</v>
       </c>
       <c r="J22" s="35" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" t="s">
         <v>101</v>
-      </c>
-      <c r="B23" t="s">
-        <v>102</v>
       </c>
       <c r="C23" s="34" t="s">
         <v>13</v>
@@ -4969,25 +4983,25 @@
       <c r="D23" s="33"/>
       <c r="E23" s="33"/>
       <c r="F23" s="33"/>
-      <c r="H23" s="106" t="s">
-        <v>52</v>
+      <c r="H23" s="108" t="s">
+        <v>51</v>
       </c>
       <c r="I23" s="34">
         <v>12</v>
       </c>
       <c r="J23" s="35" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="K23" s="35" t="s">
-        <v>39</v>
+        <v>234</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
         <v>103</v>
-      </c>
-      <c r="B24" t="s">
-        <v>104</v>
       </c>
       <c r="C24" s="34" t="s">
         <v>14</v>
@@ -4995,25 +5009,25 @@
       <c r="D24" s="33"/>
       <c r="E24" s="33"/>
       <c r="F24" s="33"/>
-      <c r="H24" s="106" t="s">
-        <v>53</v>
+      <c r="H24" s="108" t="s">
+        <v>52</v>
       </c>
       <c r="I24" s="34">
         <v>6</v>
       </c>
       <c r="J24" s="35" t="s">
-        <v>34</v>
+        <v>230</v>
       </c>
       <c r="K24" s="35" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" t="s">
         <v>105</v>
-      </c>
-      <c r="B25" t="s">
-        <v>106</v>
       </c>
       <c r="C25" s="34" t="s">
         <v>15</v>
@@ -5021,25 +5035,25 @@
       <c r="D25" s="33"/>
       <c r="E25" s="33"/>
       <c r="F25" s="33"/>
-      <c r="H25" s="106" t="s">
-        <v>54</v>
+      <c r="H25" s="108" t="s">
+        <v>53</v>
       </c>
       <c r="I25" s="34">
         <v>9</v>
       </c>
       <c r="J25" s="35" t="s">
-        <v>35</v>
+        <v>229</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" t="s">
         <v>107</v>
-      </c>
-      <c r="B26" t="s">
-        <v>108</v>
       </c>
       <c r="C26" s="34" t="s">
         <v>22</v>
@@ -5051,25 +5065,25 @@
         <v>5</v>
       </c>
       <c r="F26" s="33"/>
-      <c r="H26" s="106" t="s">
-        <v>55</v>
+      <c r="H26" s="108" t="s">
+        <v>54</v>
       </c>
       <c r="I26" s="34">
         <v>15</v>
       </c>
       <c r="J26" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" t="s">
         <v>109</v>
-      </c>
-      <c r="B27" t="s">
-        <v>110</v>
       </c>
       <c r="C27" s="34" t="s">
         <v>23</v>
@@ -5078,24 +5092,24 @@
       <c r="E27" s="33"/>
       <c r="F27" s="33"/>
       <c r="H27" s="108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I27" s="34">
         <v>16</v>
       </c>
       <c r="J27" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K27" s="35" t="s">
-        <v>39</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>110</v>
+      </c>
+      <c r="B28" t="s">
         <v>111</v>
-      </c>
-      <c r="B28" t="s">
-        <v>112</v>
       </c>
       <c r="C28" s="34" t="s">
         <v>24</v>
@@ -5104,24 +5118,24 @@
       <c r="E28" s="33"/>
       <c r="F28" s="33"/>
       <c r="H28" s="108" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I28" s="34">
         <v>7</v>
       </c>
       <c r="J28" s="35" t="s">
-        <v>34</v>
+        <v>230</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>38</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>112</v>
+      </c>
+      <c r="B29" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" t="s">
-        <v>114</v>
       </c>
       <c r="C29" s="34" t="s">
         <v>26</v>
@@ -5136,24 +5150,24 @@
         <v>28</v>
       </c>
       <c r="H29" s="108" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I29" s="34">
         <v>4</v>
       </c>
       <c r="J29" s="35" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="K29" s="35" t="s">
-        <v>39</v>
+        <v>234</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>114</v>
+      </c>
+      <c r="B30" t="s">
         <v>115</v>
-      </c>
-      <c r="B30" t="s">
-        <v>116</v>
       </c>
       <c r="C30" s="34" t="s">
         <v>29</v>
@@ -5165,105 +5179,105 @@
         <v>31</v>
       </c>
       <c r="F30" s="33"/>
-      <c r="H30" s="106" t="s">
-        <v>44</v>
+      <c r="H30" s="108" t="s">
+        <v>43</v>
       </c>
       <c r="I30" s="34">
         <v>8</v>
       </c>
       <c r="J30" s="35" t="s">
-        <v>34</v>
+        <v>230</v>
       </c>
       <c r="K30" s="35" t="s">
-        <v>39</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" t="s">
         <v>117</v>
       </c>
-      <c r="B31" t="s">
-        <v>118</v>
-      </c>
       <c r="C31" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="H31" s="106" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="H31" s="108" t="s">
+        <v>39</v>
       </c>
       <c r="I31" s="34">
         <v>5</v>
       </c>
       <c r="J31" s="35" t="s">
-        <v>34</v>
+        <v>230</v>
       </c>
       <c r="K31" s="35" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" t="s">
         <v>119</v>
       </c>
-      <c r="B32" t="s">
-        <v>120</v>
-      </c>
       <c r="C32" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="H32" s="109" t="s">
-        <v>45</v>
+        <v>56</v>
+      </c>
+      <c r="H32" s="107" t="s">
+        <v>44</v>
       </c>
       <c r="I32" s="34">
         <v>1</v>
       </c>
       <c r="J32" s="35" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="K32" s="35" t="s">
-        <v>36</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C33" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D33" t="s">
         <v>58</v>
       </c>
-      <c r="D33" t="s">
-        <v>59</v>
-      </c>
-      <c r="H33" s="109" t="s">
-        <v>46</v>
+      <c r="H33" s="107" t="s">
+        <v>45</v>
       </c>
       <c r="I33" s="34">
         <v>14</v>
       </c>
       <c r="J33" s="35" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="K33" s="35" t="s">
-        <v>37</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" t="s">
         <v>122</v>
-      </c>
-      <c r="B34" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>123</v>
+      </c>
+      <c r="B35" t="s">
         <v>124</v>
-      </c>
-      <c r="B35" t="s">
-        <v>125</v>
       </c>
       <c r="C35" t="s">
         <v>32</v>
@@ -5271,282 +5285,282 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" t="s">
         <v>126</v>
-      </c>
-      <c r="B36" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" t="s">
         <v>128</v>
-      </c>
-      <c r="B37" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" t="s">
         <v>130</v>
-      </c>
-      <c r="B38" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" t="s">
         <v>132</v>
-      </c>
-      <c r="B39" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>133</v>
+      </c>
+      <c r="B40" t="s">
         <v>134</v>
-      </c>
-      <c r="B40" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" t="s">
         <v>136</v>
-      </c>
-      <c r="B41" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" t="s">
         <v>138</v>
-      </c>
-      <c r="B42" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>139</v>
+      </c>
+      <c r="B43" t="s">
         <v>140</v>
-      </c>
-      <c r="B43" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>141</v>
+      </c>
+      <c r="B44" t="s">
         <v>142</v>
-      </c>
-      <c r="B44" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
         <v>144</v>
-      </c>
-      <c r="B45" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>145</v>
+      </c>
+      <c r="B46" t="s">
         <v>146</v>
-      </c>
-      <c r="B46" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B47" t="s">
         <v>148</v>
-      </c>
-      <c r="B47" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>149</v>
+      </c>
+      <c r="B48" t="s">
         <v>150</v>
-      </c>
-      <c r="B48" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>151</v>
+      </c>
+      <c r="B49" t="s">
         <v>152</v>
-      </c>
-      <c r="B49" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>153</v>
+      </c>
+      <c r="B50" t="s">
         <v>154</v>
-      </c>
-      <c r="B50" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>155</v>
+      </c>
+      <c r="B51" t="s">
         <v>156</v>
-      </c>
-      <c r="B51" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" t="s">
         <v>158</v>
-      </c>
-      <c r="B52" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>159</v>
+      </c>
+      <c r="B53" t="s">
         <v>160</v>
-      </c>
-      <c r="B53" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" t="s">
         <v>162</v>
-      </c>
-      <c r="B54" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>163</v>
+      </c>
+      <c r="B55" t="s">
         <v>164</v>
-      </c>
-      <c r="B55" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" t="s">
         <v>166</v>
-      </c>
-      <c r="B56" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>167</v>
+      </c>
+      <c r="B57" t="s">
         <v>168</v>
-      </c>
-      <c r="B57" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>169</v>
+      </c>
+      <c r="B58" t="s">
         <v>170</v>
-      </c>
-      <c r="B58" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
+        <v>171</v>
+      </c>
+      <c r="B59" t="s">
         <v>172</v>
-      </c>
-      <c r="B59" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>173</v>
+      </c>
+      <c r="B60" t="s">
         <v>174</v>
-      </c>
-      <c r="B60" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>175</v>
+      </c>
+      <c r="B61" t="s">
         <v>176</v>
-      </c>
-      <c r="B61" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>177</v>
+      </c>
+      <c r="B62" t="s">
         <v>178</v>
-      </c>
-      <c r="B62" t="s">
-        <v>179</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>179</v>
+      </c>
+      <c r="B63" t="s">
         <v>180</v>
-      </c>
-      <c r="B63" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>181</v>
+      </c>
+      <c r="B64" t="s">
         <v>182</v>
-      </c>
-      <c r="B64" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
+        <v>183</v>
+      </c>
+      <c r="B65" t="s">
         <v>184</v>
-      </c>
-      <c r="B65" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>185</v>
+      </c>
+      <c r="B66" t="s">
         <v>186</v>
-      </c>
-      <c r="B66" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" t="s">
         <v>188</v>
-      </c>
-      <c r="B67" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>189</v>
+      </c>
+      <c r="B68" t="s">
         <v>190</v>
-      </c>
-      <c r="B68" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>191</v>
+      </c>
+      <c r="B69" t="s">
         <v>192</v>
-      </c>
-      <c r="B69" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>193</v>
+      </c>
+      <c r="B70" t="s">
         <v>194</v>
-      </c>
-      <c r="B70" t="s">
-        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -5580,122 +5594,122 @@
   <sheetData>
     <row r="2" spans="2:6" s="105" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="B2" s="104" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D2" s="104" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F2" s="104" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="2:6" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B3" s="104" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="104" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F3" s="104" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="4" spans="2:6" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B4" s="104" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="104" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F4" s="104" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="2:6" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B5" s="104" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" s="104" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F5" s="104" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B6" s="104" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" s="104" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F6" s="104" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="2:6" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B7" s="104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D7" s="104" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F7" s="104" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="2:6" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B8" s="104" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D8" s="104" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F8" s="104" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="2:6" s="105" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="B9" s="104" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" s="104" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="F9" s="104" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="2:6" s="105" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B10" s="104" t="s">
+        <v>203</v>
+      </c>
+      <c r="D10" s="104" t="s">
         <v>204</v>
       </c>
-      <c r="D10" s="104" t="s">
-        <v>205</v>
-      </c>
       <c r="F10" s="104" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="2:6" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B11" s="104" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="104" t="s">
         <v>205</v>
-      </c>
-      <c r="D11" s="104" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="12" spans="2:6" s="105" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B12" s="104" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D12" s="104" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" spans="2:6" s="105" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B13" s="104" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="2:6" s="105" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Lighting and level design
</commit_message>
<xml_diff>
--- a/Assets/Documents/Game Document.xlsx
+++ b/Assets/Documents/Game Document.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\Horror_FPS\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AD079A-407E-48E9-B596-C94AA9017F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05EF363F-CD25-4B67-85E6-931C4210E2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nursery_big" sheetId="6" r:id="rId1"/>
     <sheet name="Items" sheetId="5" r:id="rId2"/>
-    <sheet name="Gameplay flow" sheetId="8" r:id="rId3"/>
-    <sheet name="story" sheetId="7" r:id="rId4"/>
-    <sheet name="Floor Texture" sheetId="4" r:id="rId5"/>
+    <sheet name="Gameplay flow description" sheetId="8" r:id="rId3"/>
+    <sheet name="Gameplay Flow" sheetId="9" r:id="rId4"/>
+    <sheet name="story" sheetId="7" r:id="rId5"/>
+    <sheet name="Floor Texture" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$H$17:$K$33</definedName>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="259">
   <si>
     <t>Item</t>
   </si>
@@ -815,7 +816,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -840,6 +841,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1291,7 +1299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1605,6 +1613,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1630,6 +1641,1720 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>272142</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Conector: angular 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711DFAFC-B1D8-7E54-3150-058650349281}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3876675" y="2524125"/>
+          <a:ext cx="1538967" cy="1353911"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 74138"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>160734</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>163286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>160734</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Conector recto 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F30FDA62-C088-1D01-BA26-3A3765AEF3ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14733984" y="2449286"/>
+          <a:ext cx="2552" cy="1711948"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>136071</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>163286</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="Conector recto 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1A1767-EAE8-C126-F282-00C485F6BAE7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13280571" y="4150179"/>
+          <a:ext cx="1455965" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>148828</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>149679</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>196453</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Conector recto 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE75105F-5038-A32D-59C0-91BE1222DA69}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="13293328" y="4150179"/>
+          <a:ext cx="851" cy="1189774"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>184547</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>160734</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>204107</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Conector recto 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A174142-F93A-97F1-5D56-BC7B4820F608}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5238750" y="5328047"/>
+          <a:ext cx="8066484" cy="19560"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>226219</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>107156</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>214312</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Conector recto 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24C53F58-2C1C-BF7F-67A6-2F996551996F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5238750" y="3940969"/>
+          <a:ext cx="11906" cy="1416843"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>231321</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>231321</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="40" name="Conector recto 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B563E933-3305-C976-D01A-6EFDB7D1FD70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238750" y="3946071"/>
+          <a:ext cx="830036" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>176893</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>176893</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Conector recto de flecha 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02C786B-2502-054E-EE28-3FA5C01C4114}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="14069786" y="2462893"/>
+          <a:ext cx="680357" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266704</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="61" name="Conector: angular 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AA279DC-9447-1339-2D54-16662D29BA97}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000" flipV="1">
+          <a:off x="4552954" y="5572125"/>
+          <a:ext cx="8839196" cy="1162050"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 98060"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>239184</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>239184</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Conector recto 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A89774-74F0-8E94-A964-218D87A0C69D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="13383684" y="4552950"/>
+          <a:ext cx="0" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>247650</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="73" name="Conector recto de flecha 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33574CF7-C51D-0808-E350-CE01C347A03E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4591050" y="6819900"/>
+          <a:ext cx="552450" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>59531</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="78" name="Conector recto 77">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72837085-56AA-AD49-41F6-A3C55E63BFF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5000625" y="5715000"/>
+          <a:ext cx="8203406" cy="5953"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>276225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Conector recto 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88603D43-5B4E-FB59-49C1-F6265EDA12B0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5010150" y="5705475"/>
+          <a:ext cx="0" cy="962025"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="Conector recto 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F84181-2698-0464-FEC8-D63C6321AACF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5010150" y="6667500"/>
+          <a:ext cx="133350" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>5953</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Conector recto de flecha 90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9882E70A-D5E9-F0B1-2277-DC9793FD65E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13192125" y="5720953"/>
+          <a:ext cx="0" cy="285750"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>209551</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="104" name="Conector: angular 103">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54AECD39-7FF0-D568-8DCD-04A7074BCD80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="4552950" y="3857628"/>
+          <a:ext cx="8743950" cy="1781173"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 96514"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="Conector recto 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296A9834-7F51-F21B-53E4-3B3B06E3A150}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13296900" y="5638800"/>
+          <a:ext cx="0" cy="361950"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>228600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>147205</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>60614</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="114" name="Conector: angular 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F67CE7-F5C8-ACB0-C802-381702C6F4B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4581525" y="3943350"/>
+          <a:ext cx="2995180" cy="1546514"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 12128"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>121227</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>138545</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>8659</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="117" name="Conector recto de flecha 116">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090E81F0-443E-6918-54B2-42919F5D96D8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7550727" y="5481205"/>
+          <a:ext cx="17318" cy="528204"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="123" name="Conector recto 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577D3501-9328-F5EC-080B-DE787E7551BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="7667625" y="5838825"/>
+          <a:ext cx="2714625" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="125" name="Conector recto de flecha 124">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D5FEE7-92C5-D139-F653-230A3E01F91E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10382250" y="4543425"/>
+          <a:ext cx="0" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>234950</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>279400</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="127" name="Conector recto 126">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{850DE473-F646-5DB9-9469-7F1E8FCF7259}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7664450" y="5842000"/>
+          <a:ext cx="0" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>181841</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>8659</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>199159</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="132" name="Conector recto de flecha 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04063B44-D720-9CC2-C736-29613F51A4FD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="10468841" y="4580659"/>
+          <a:ext cx="17318" cy="1420091"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>51955</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>60614</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="140" name="Conector recto 139">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{361D4E4E-8242-6C2C-DFF9-19A39C9082E4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="10338955" y="5143500"/>
+          <a:ext cx="8659" cy="857250"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>60614</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>8659</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="142" name="Conector recto 141">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC83A31B-A200-55E0-3F0E-2341489ED50A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="5134841" y="5143500"/>
+          <a:ext cx="5212773" cy="8659"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>8659</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="144" name="Conector recto 143">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C65928E1-493D-61D1-DFAC-9CECAD98E827}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5134841" y="2441864"/>
+          <a:ext cx="0" cy="2710295"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>277091</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>8659</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="146" name="Conector recto de flecha 145">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23DFFBB-6CFC-3A68-62EC-58AB42F1D419}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5134841" y="2441864"/>
+          <a:ext cx="303068" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>138545</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>43295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>138545</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="155" name="Conector recto 154">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253621EA-18D1-B30C-8E68-1EC6806979FA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4710545" y="2329295"/>
+          <a:ext cx="0" cy="2970069"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>268432</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>147205</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>138545</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>155864</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="159" name="Conector recto de flecha 158">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A4666A-55E7-0490-41DF-625F9FDC464C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="4554682" y="5290705"/>
+          <a:ext cx="155863" cy="8659"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>129886</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>43295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>51955</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="161" name="Conector recto 160">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DE25EA7-44D2-25DB-74A3-14A3ADBEAE89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4701886" y="2329295"/>
+          <a:ext cx="727364" cy="8660"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1897,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9E5FAB-1047-4072-92C4-3E2647FF44F0}">
   <dimension ref="I1:CJ689"/>
   <sheetViews>
-    <sheetView topLeftCell="I4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4685,8 +6410,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A7:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5703,7 +7428,7 @@
   <dimension ref="C2:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5727,7 +7452,7 @@
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="108" t="s">
+      <c r="C5" s="109" t="s">
         <v>224</v>
       </c>
     </row>
@@ -5835,6 +7560,2794 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05D0279-7390-4F74-B85A-28B109ED7871}">
+  <dimension ref="A1:CB689"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X23" sqref="X23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="83" width="4.28515625" style="1" customWidth="1"/>
+    <col min="84" max="16384" width="11.42578125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:80" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>4</v>
+      </c>
+      <c r="K6" s="1">
+        <v>5</v>
+      </c>
+      <c r="L6" s="1">
+        <v>6</v>
+      </c>
+      <c r="M6" s="1">
+        <v>7</v>
+      </c>
+      <c r="N6" s="1">
+        <v>8</v>
+      </c>
+      <c r="O6" s="1">
+        <v>9</v>
+      </c>
+      <c r="P6" s="1">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="1">
+        <v>11</v>
+      </c>
+      <c r="R6" s="1">
+        <v>12</v>
+      </c>
+      <c r="S6" s="1">
+        <v>13</v>
+      </c>
+      <c r="T6" s="1">
+        <v>14</v>
+      </c>
+      <c r="U6" s="1">
+        <v>15</v>
+      </c>
+      <c r="V6" s="1">
+        <v>16</v>
+      </c>
+      <c r="W6" s="1">
+        <v>17</v>
+      </c>
+      <c r="X6" s="1">
+        <v>18</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>19</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>20</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>21</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>22</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>24</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>25</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>26</v>
+      </c>
+      <c r="AG6" s="1">
+        <v>27</v>
+      </c>
+      <c r="AH6" s="1">
+        <v>28</v>
+      </c>
+      <c r="AI6" s="1">
+        <v>29</v>
+      </c>
+      <c r="AJ6" s="1">
+        <v>30</v>
+      </c>
+      <c r="AK6" s="1">
+        <v>31</v>
+      </c>
+      <c r="AL6" s="1">
+        <v>32</v>
+      </c>
+      <c r="AM6" s="1">
+        <v>33</v>
+      </c>
+      <c r="AN6" s="1">
+        <v>34</v>
+      </c>
+      <c r="AO6" s="1">
+        <v>35</v>
+      </c>
+      <c r="AP6" s="1">
+        <v>36</v>
+      </c>
+      <c r="AQ6" s="1">
+        <v>37</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>38</v>
+      </c>
+      <c r="AS6" s="1">
+        <v>39</v>
+      </c>
+      <c r="AT6" s="1">
+        <v>40</v>
+      </c>
+      <c r="AU6" s="1">
+        <v>41</v>
+      </c>
+      <c r="AV6" s="1">
+        <v>42</v>
+      </c>
+      <c r="AW6" s="1">
+        <v>43</v>
+      </c>
+      <c r="AX6" s="1">
+        <v>44</v>
+      </c>
+      <c r="AY6" s="1">
+        <v>45</v>
+      </c>
+      <c r="AZ6" s="1">
+        <v>46</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>47</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>48</v>
+      </c>
+      <c r="BC6" s="1">
+        <v>49</v>
+      </c>
+      <c r="BD6" s="1">
+        <v>50</v>
+      </c>
+      <c r="BE6" s="1">
+        <v>51</v>
+      </c>
+      <c r="BF6" s="1">
+        <v>52</v>
+      </c>
+      <c r="BG6" s="1">
+        <v>53</v>
+      </c>
+      <c r="BH6" s="1">
+        <v>54</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>55</v>
+      </c>
+      <c r="BJ6" s="1">
+        <v>56</v>
+      </c>
+      <c r="BK6" s="1">
+        <v>57</v>
+      </c>
+      <c r="BL6" s="1">
+        <v>58</v>
+      </c>
+      <c r="BM6" s="1">
+        <v>59</v>
+      </c>
+      <c r="BN6" s="1">
+        <v>60</v>
+      </c>
+      <c r="BO6" s="1">
+        <v>61</v>
+      </c>
+      <c r="BP6" s="1">
+        <v>62</v>
+      </c>
+      <c r="BQ6" s="1">
+        <v>63</v>
+      </c>
+      <c r="BR6" s="1">
+        <v>64</v>
+      </c>
+      <c r="BS6" s="1">
+        <v>65</v>
+      </c>
+      <c r="BT6" s="1">
+        <v>66</v>
+      </c>
+      <c r="BU6" s="1">
+        <v>67</v>
+      </c>
+      <c r="BV6" s="1">
+        <v>68</v>
+      </c>
+      <c r="BW6" s="1">
+        <v>69</v>
+      </c>
+      <c r="BX6" s="1">
+        <v>70</v>
+      </c>
+      <c r="BY6" s="1">
+        <v>71</v>
+      </c>
+      <c r="BZ6" s="1">
+        <v>72</v>
+      </c>
+      <c r="CA6" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="L7" s="7"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="39"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="9"/>
+      <c r="Y7" s="40"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="41"/>
+      <c r="AB7" s="41"/>
+      <c r="AC7" s="41"/>
+      <c r="AD7" s="41"/>
+      <c r="AE7" s="41"/>
+      <c r="AF7" s="41"/>
+      <c r="AG7" s="41"/>
+      <c r="AH7" s="42"/>
+      <c r="AI7" s="40"/>
+      <c r="AJ7" s="41"/>
+      <c r="AK7" s="41"/>
+      <c r="AL7" s="41"/>
+      <c r="AM7" s="41"/>
+      <c r="AN7" s="41"/>
+      <c r="AO7" s="41"/>
+      <c r="AP7" s="41"/>
+      <c r="AQ7" s="41"/>
+      <c r="AR7" s="42"/>
+      <c r="AS7" s="43"/>
+      <c r="AT7" s="44"/>
+      <c r="AU7" s="44"/>
+      <c r="AV7" s="44"/>
+      <c r="AW7" s="45"/>
+      <c r="AX7" s="46"/>
+      <c r="AY7" s="47"/>
+      <c r="AZ7" s="47"/>
+      <c r="BA7" s="47"/>
+      <c r="BB7" s="48"/>
+      <c r="BC7" s="37"/>
+      <c r="BD7" s="38"/>
+      <c r="BE7" s="38"/>
+      <c r="BF7" s="38"/>
+      <c r="BG7" s="38"/>
+      <c r="BH7" s="38"/>
+      <c r="BI7" s="38"/>
+      <c r="BJ7" s="38"/>
+      <c r="BK7" s="38"/>
+      <c r="BL7" s="38"/>
+      <c r="BM7" s="38"/>
+      <c r="BN7" s="38"/>
+      <c r="BO7" s="38"/>
+      <c r="BP7" s="38"/>
+      <c r="BQ7" s="38"/>
+      <c r="BR7" s="38"/>
+      <c r="BS7" s="38"/>
+      <c r="BT7" s="38"/>
+      <c r="BU7" s="38"/>
+      <c r="BV7" s="38"/>
+      <c r="BW7" s="38"/>
+      <c r="BX7" s="38"/>
+      <c r="BY7" s="38"/>
+      <c r="BZ7" s="38"/>
+      <c r="CA7" s="39"/>
+      <c r="CB7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K8" s="2"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="10"/>
+      <c r="U8" s="11"/>
+      <c r="V8" s="11"/>
+      <c r="W8" s="11"/>
+      <c r="X8" s="16"/>
+      <c r="Y8" s="52"/>
+      <c r="Z8" s="53"/>
+      <c r="AA8" s="53"/>
+      <c r="AB8" s="53"/>
+      <c r="AC8" s="53"/>
+      <c r="AD8" s="53"/>
+      <c r="AE8" s="53"/>
+      <c r="AF8" s="53"/>
+      <c r="AG8" s="53"/>
+      <c r="AH8" s="54"/>
+      <c r="AI8" s="52"/>
+      <c r="AJ8" s="53"/>
+      <c r="AK8" s="53"/>
+      <c r="AL8" s="53"/>
+      <c r="AM8" s="53"/>
+      <c r="AN8" s="53"/>
+      <c r="AO8" s="53"/>
+      <c r="AP8" s="53"/>
+      <c r="AQ8" s="53"/>
+      <c r="AR8" s="54"/>
+      <c r="AS8" s="55"/>
+      <c r="AT8" s="56"/>
+      <c r="AU8" s="56"/>
+      <c r="AV8" s="56"/>
+      <c r="AW8" s="57"/>
+      <c r="AX8" s="58"/>
+      <c r="AY8" s="59"/>
+      <c r="AZ8" s="59"/>
+      <c r="BA8" s="59"/>
+      <c r="BB8" s="60"/>
+      <c r="BC8" s="61"/>
+      <c r="BD8" s="50"/>
+      <c r="BE8" s="50"/>
+      <c r="BF8" s="50"/>
+      <c r="BG8" s="50"/>
+      <c r="BH8" s="50"/>
+      <c r="BI8" s="50"/>
+      <c r="BJ8" s="50"/>
+      <c r="BK8" s="50"/>
+      <c r="BL8" s="50"/>
+      <c r="BM8" s="50"/>
+      <c r="BN8" s="50"/>
+      <c r="BO8" s="50"/>
+      <c r="BP8" s="50"/>
+      <c r="BQ8" s="50"/>
+      <c r="BR8" s="50"/>
+      <c r="BS8" s="50"/>
+      <c r="BT8" s="50"/>
+      <c r="BU8" s="50"/>
+      <c r="BV8" s="50"/>
+      <c r="BW8" s="50"/>
+      <c r="BX8" s="50"/>
+      <c r="BY8" s="50"/>
+      <c r="BZ8" s="50"/>
+      <c r="CA8" s="62"/>
+      <c r="CB8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="O9" s="11"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="49"/>
+      <c r="R9" s="50"/>
+      <c r="S9" s="51"/>
+      <c r="T9" s="12"/>
+      <c r="U9" s="11"/>
+      <c r="V9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="W9" s="11"/>
+      <c r="X9" s="16"/>
+      <c r="Y9" s="52"/>
+      <c r="Z9" s="53"/>
+      <c r="AA9" s="53"/>
+      <c r="AB9" s="53"/>
+      <c r="AC9" s="53"/>
+      <c r="AD9" s="53"/>
+      <c r="AE9" s="53"/>
+      <c r="AF9" s="53"/>
+      <c r="AG9" s="53"/>
+      <c r="AH9" s="54"/>
+      <c r="AI9" s="52"/>
+      <c r="AJ9" s="53"/>
+      <c r="AK9" s="53"/>
+      <c r="AL9" s="53"/>
+      <c r="AM9" s="53"/>
+      <c r="AN9" s="53"/>
+      <c r="AO9" s="53"/>
+      <c r="AP9" s="53"/>
+      <c r="AQ9" s="53"/>
+      <c r="AR9" s="54"/>
+      <c r="AS9" s="55"/>
+      <c r="AT9" s="56"/>
+      <c r="AU9" s="56" t="s">
+        <v>45</v>
+      </c>
+      <c r="AV9" s="56"/>
+      <c r="AW9" s="63"/>
+      <c r="AX9" s="58"/>
+      <c r="AY9" s="59"/>
+      <c r="AZ9" s="59"/>
+      <c r="BA9" s="59"/>
+      <c r="BB9" s="60"/>
+      <c r="BC9" s="61"/>
+      <c r="BD9" s="50"/>
+      <c r="BE9" s="50"/>
+      <c r="BF9" s="50"/>
+      <c r="BG9" s="50"/>
+      <c r="BH9" s="50"/>
+      <c r="BI9" s="50"/>
+      <c r="BJ9" s="50"/>
+      <c r="BK9" s="50"/>
+      <c r="BL9" s="50"/>
+      <c r="BM9" s="50"/>
+      <c r="BN9" s="50"/>
+      <c r="BO9" s="50"/>
+      <c r="BP9" s="50"/>
+      <c r="BQ9" s="50"/>
+      <c r="BR9" s="50"/>
+      <c r="BS9" s="50"/>
+      <c r="BT9" s="50"/>
+      <c r="BU9" s="50"/>
+      <c r="BV9" s="50"/>
+      <c r="BW9" s="50"/>
+      <c r="BX9" s="50"/>
+      <c r="BY9" s="50"/>
+      <c r="BZ9" s="50"/>
+      <c r="CA9" s="62"/>
+      <c r="CB9" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K10" s="2"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="49"/>
+      <c r="R10" s="50"/>
+      <c r="S10" s="51"/>
+      <c r="T10" s="10"/>
+      <c r="U10" s="11"/>
+      <c r="V10" s="11"/>
+      <c r="W10" s="11"/>
+      <c r="X10" s="16"/>
+      <c r="Y10" s="52"/>
+      <c r="Z10" s="53"/>
+      <c r="AA10" s="53"/>
+      <c r="AB10" s="53"/>
+      <c r="AC10" s="53"/>
+      <c r="AD10" s="53"/>
+      <c r="AE10" s="53"/>
+      <c r="AF10" s="53"/>
+      <c r="AG10" s="53"/>
+      <c r="AH10" s="54"/>
+      <c r="AI10" s="52"/>
+      <c r="AJ10" s="53"/>
+      <c r="AK10" s="53"/>
+      <c r="AL10" s="53"/>
+      <c r="AM10" s="53"/>
+      <c r="AN10" s="53"/>
+      <c r="AO10" s="53"/>
+      <c r="AP10" s="53"/>
+      <c r="AQ10" s="53"/>
+      <c r="AR10" s="54"/>
+      <c r="AS10" s="55"/>
+      <c r="AT10" s="56"/>
+      <c r="AU10" s="56"/>
+      <c r="AV10" s="56"/>
+      <c r="AW10" s="57"/>
+      <c r="AX10" s="58"/>
+      <c r="AY10" s="59"/>
+      <c r="AZ10" s="59"/>
+      <c r="BA10" s="59"/>
+      <c r="BB10" s="60"/>
+      <c r="BC10" s="61"/>
+      <c r="BD10" s="50"/>
+      <c r="BE10" s="50"/>
+      <c r="BF10" s="50"/>
+      <c r="BG10" s="50"/>
+      <c r="BH10" s="50"/>
+      <c r="BI10" s="50"/>
+      <c r="BJ10" s="50"/>
+      <c r="BK10" s="50"/>
+      <c r="BL10" s="50"/>
+      <c r="BM10" s="50"/>
+      <c r="BN10" s="50"/>
+      <c r="BO10" s="50"/>
+      <c r="BP10" s="50"/>
+      <c r="BQ10" s="50"/>
+      <c r="BR10" s="50"/>
+      <c r="BS10" s="50"/>
+      <c r="BT10" s="50"/>
+      <c r="BU10" s="50"/>
+      <c r="BV10" s="50"/>
+      <c r="BW10" s="50"/>
+      <c r="BX10" s="50"/>
+      <c r="BY10" s="50"/>
+      <c r="BZ10" s="50"/>
+      <c r="CA10" s="62"/>
+      <c r="CB10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:80" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K11" s="2"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="14"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="50"/>
+      <c r="S11" s="51"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="52"/>
+      <c r="Z11" s="53"/>
+      <c r="AA11" s="53"/>
+      <c r="AB11" s="53"/>
+      <c r="AC11" s="53" t="s">
+        <v>46</v>
+      </c>
+      <c r="AD11" s="53"/>
+      <c r="AE11" s="53"/>
+      <c r="AF11" s="53"/>
+      <c r="AG11" s="53"/>
+      <c r="AH11" s="54"/>
+      <c r="AI11" s="52"/>
+      <c r="AJ11" s="53"/>
+      <c r="AK11" s="53"/>
+      <c r="AL11" s="53"/>
+      <c r="AM11" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="AN11" s="53"/>
+      <c r="AO11" s="53"/>
+      <c r="AP11" s="53"/>
+      <c r="AQ11" s="53"/>
+      <c r="AR11" s="54"/>
+      <c r="AS11" s="64"/>
+      <c r="AT11" s="65"/>
+      <c r="AU11" s="65"/>
+      <c r="AV11" s="65"/>
+      <c r="AW11" s="66"/>
+      <c r="AX11" s="58"/>
+      <c r="AY11" s="59"/>
+      <c r="AZ11" s="59"/>
+      <c r="BA11" s="59"/>
+      <c r="BB11" s="60"/>
+      <c r="BC11" s="61"/>
+      <c r="BD11" s="50"/>
+      <c r="BE11" s="50"/>
+      <c r="BF11" s="50"/>
+      <c r="BG11" s="50"/>
+      <c r="BH11" s="50"/>
+      <c r="BI11" s="50"/>
+      <c r="BJ11" s="50"/>
+      <c r="BK11" s="50"/>
+      <c r="BL11" s="50"/>
+      <c r="BM11" s="50"/>
+      <c r="BN11" s="50"/>
+      <c r="BO11" s="50"/>
+      <c r="BP11" s="50"/>
+      <c r="BQ11" s="50"/>
+      <c r="BR11" s="50"/>
+      <c r="BS11" s="50"/>
+      <c r="BT11" s="50"/>
+      <c r="BU11" s="50"/>
+      <c r="BV11" s="50"/>
+      <c r="BW11" s="50"/>
+      <c r="BX11" s="50"/>
+      <c r="BY11" s="50"/>
+      <c r="BZ11" s="50"/>
+      <c r="CA11" s="62"/>
+      <c r="CB11" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="2"/>
+      <c r="L12" s="7"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="52"/>
+      <c r="Z12" s="53"/>
+      <c r="AA12" s="53"/>
+      <c r="AB12" s="53"/>
+      <c r="AC12" s="53"/>
+      <c r="AD12" s="53"/>
+      <c r="AE12" s="53"/>
+      <c r="AF12" s="53"/>
+      <c r="AG12" s="53"/>
+      <c r="AH12" s="54"/>
+      <c r="AI12" s="52"/>
+      <c r="AJ12" s="53"/>
+      <c r="AK12" s="53"/>
+      <c r="AL12" s="53"/>
+      <c r="AM12" s="53"/>
+      <c r="AN12" s="53"/>
+      <c r="AO12" s="53"/>
+      <c r="AP12" s="53"/>
+      <c r="AQ12" s="53"/>
+      <c r="AR12" s="54"/>
+      <c r="AS12" s="67"/>
+      <c r="AT12" s="68"/>
+      <c r="AU12" s="68"/>
+      <c r="AV12" s="68"/>
+      <c r="AW12" s="68"/>
+      <c r="AX12" s="59"/>
+      <c r="AY12" s="59"/>
+      <c r="AZ12" s="59"/>
+      <c r="BA12" s="59"/>
+      <c r="BB12" s="60"/>
+      <c r="BC12" s="61"/>
+      <c r="BD12" s="50"/>
+      <c r="BE12" s="50"/>
+      <c r="BF12" s="50"/>
+      <c r="BG12" s="50"/>
+      <c r="BH12" s="50"/>
+      <c r="BI12" s="50"/>
+      <c r="BJ12" s="50"/>
+      <c r="BK12" s="50"/>
+      <c r="BL12" s="50"/>
+      <c r="BM12" s="50"/>
+      <c r="BN12" s="50"/>
+      <c r="BO12" s="50"/>
+      <c r="BP12" s="50"/>
+      <c r="BQ12" s="50"/>
+      <c r="BR12" s="50"/>
+      <c r="BS12" s="50"/>
+      <c r="BT12" s="50"/>
+      <c r="BU12" s="50"/>
+      <c r="BV12" s="50"/>
+      <c r="BW12" s="50"/>
+      <c r="BX12" s="50"/>
+      <c r="BY12" s="50"/>
+      <c r="BZ12" s="50"/>
+      <c r="CA12" s="62"/>
+      <c r="CB12" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K13" s="2"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="11"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="49"/>
+      <c r="R13" s="50"/>
+      <c r="S13" s="51"/>
+      <c r="T13" s="10"/>
+      <c r="U13" s="11"/>
+      <c r="V13" s="11"/>
+      <c r="W13" s="11"/>
+      <c r="X13" s="16"/>
+      <c r="Y13" s="52"/>
+      <c r="Z13" s="53"/>
+      <c r="AA13" s="53"/>
+      <c r="AB13" s="53"/>
+      <c r="AC13" s="53"/>
+      <c r="AD13" s="53"/>
+      <c r="AE13" s="53"/>
+      <c r="AF13" s="53"/>
+      <c r="AG13" s="53"/>
+      <c r="AH13" s="54"/>
+      <c r="AI13" s="52"/>
+      <c r="AJ13" s="53"/>
+      <c r="AK13" s="53"/>
+      <c r="AL13" s="53"/>
+      <c r="AM13" s="53"/>
+      <c r="AN13" s="53"/>
+      <c r="AO13" s="53"/>
+      <c r="AP13" s="53"/>
+      <c r="AQ13" s="53"/>
+      <c r="AR13" s="54"/>
+      <c r="AS13" s="69"/>
+      <c r="AT13" s="59"/>
+      <c r="AU13" s="59"/>
+      <c r="AV13" s="59"/>
+      <c r="AW13" s="59" t="s">
+        <v>50</v>
+      </c>
+      <c r="AX13" s="59"/>
+      <c r="AY13" s="59"/>
+      <c r="AZ13" s="59"/>
+      <c r="BA13" s="59"/>
+      <c r="BB13" s="60"/>
+      <c r="BC13" s="61"/>
+      <c r="BD13" s="50"/>
+      <c r="BE13" s="50"/>
+      <c r="BF13" s="50"/>
+      <c r="BG13" s="50"/>
+      <c r="BH13" s="50"/>
+      <c r="BI13" s="50"/>
+      <c r="BJ13" s="50"/>
+      <c r="BK13" s="50"/>
+      <c r="BL13" s="50"/>
+      <c r="BM13" s="50"/>
+      <c r="BN13" s="50"/>
+      <c r="BO13" s="50"/>
+      <c r="BP13" s="50"/>
+      <c r="BQ13" s="50"/>
+      <c r="BR13" s="50"/>
+      <c r="BS13" s="50"/>
+      <c r="BT13" s="50"/>
+      <c r="BU13" s="50"/>
+      <c r="BV13" s="50"/>
+      <c r="BW13" s="50"/>
+      <c r="BX13" s="50"/>
+      <c r="BY13" s="50"/>
+      <c r="BZ13" s="50"/>
+      <c r="CA13" s="62"/>
+      <c r="CB13" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="O14" s="11"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="50"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="W14" s="11"/>
+      <c r="X14" s="16"/>
+      <c r="Y14" s="52"/>
+      <c r="Z14" s="53"/>
+      <c r="AA14" s="53"/>
+      <c r="AB14" s="53"/>
+      <c r="AC14" s="53"/>
+      <c r="AD14" s="53"/>
+      <c r="AE14" s="53"/>
+      <c r="AF14" s="53"/>
+      <c r="AG14" s="53"/>
+      <c r="AH14" s="54"/>
+      <c r="AI14" s="52"/>
+      <c r="AJ14" s="53"/>
+      <c r="AK14" s="53"/>
+      <c r="AL14" s="53"/>
+      <c r="AM14" s="53"/>
+      <c r="AN14" s="53"/>
+      <c r="AO14" s="53"/>
+      <c r="AP14" s="53"/>
+      <c r="AQ14" s="53"/>
+      <c r="AR14" s="54"/>
+      <c r="AS14" s="69"/>
+      <c r="AT14" s="59"/>
+      <c r="AU14" s="59"/>
+      <c r="AV14" s="59"/>
+      <c r="AW14" s="59"/>
+      <c r="AX14" s="59"/>
+      <c r="AY14" s="59"/>
+      <c r="AZ14" s="59"/>
+      <c r="BA14" s="59"/>
+      <c r="BB14" s="60"/>
+      <c r="BC14" s="61"/>
+      <c r="BD14" s="50"/>
+      <c r="BE14" s="50"/>
+      <c r="BF14" s="50"/>
+      <c r="BG14" s="50"/>
+      <c r="BH14" s="50"/>
+      <c r="BI14" s="50"/>
+      <c r="BJ14" s="50"/>
+      <c r="BK14" s="50"/>
+      <c r="BL14" s="50"/>
+      <c r="BM14" s="50"/>
+      <c r="BN14" s="50"/>
+      <c r="BO14" s="50"/>
+      <c r="BP14" s="50"/>
+      <c r="BQ14" s="50"/>
+      <c r="BR14" s="50"/>
+      <c r="BS14" s="50"/>
+      <c r="BT14" s="50"/>
+      <c r="BU14" s="50"/>
+      <c r="BV14" s="50"/>
+      <c r="BW14" s="50"/>
+      <c r="BX14" s="50"/>
+      <c r="BY14" s="50"/>
+      <c r="BZ14" s="50"/>
+      <c r="CA14" s="62"/>
+      <c r="CB14" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="2:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="2"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="10"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="16"/>
+      <c r="Y15" s="52"/>
+      <c r="Z15" s="53"/>
+      <c r="AA15" s="53"/>
+      <c r="AB15" s="53"/>
+      <c r="AC15" s="53"/>
+      <c r="AD15" s="53"/>
+      <c r="AE15" s="53"/>
+      <c r="AF15" s="53"/>
+      <c r="AG15" s="53"/>
+      <c r="AH15" s="54"/>
+      <c r="AI15" s="52"/>
+      <c r="AJ15" s="53"/>
+      <c r="AK15" s="53"/>
+      <c r="AL15" s="53"/>
+      <c r="AM15" s="53"/>
+      <c r="AN15" s="53"/>
+      <c r="AO15" s="53"/>
+      <c r="AP15" s="53"/>
+      <c r="AQ15" s="53"/>
+      <c r="AR15" s="54"/>
+      <c r="AS15" s="69"/>
+      <c r="AT15" s="59"/>
+      <c r="AU15" s="59"/>
+      <c r="AV15" s="59"/>
+      <c r="AW15" s="59"/>
+      <c r="AX15" s="59"/>
+      <c r="AY15" s="59"/>
+      <c r="AZ15" s="59"/>
+      <c r="BA15" s="59"/>
+      <c r="BB15" s="60"/>
+      <c r="BC15" s="61"/>
+      <c r="BD15" s="50"/>
+      <c r="BE15" s="50"/>
+      <c r="BF15" s="50"/>
+      <c r="BG15" s="50"/>
+      <c r="BH15" s="50"/>
+      <c r="BI15" s="50"/>
+      <c r="BJ15" s="50"/>
+      <c r="BK15" s="50"/>
+      <c r="BL15" s="50"/>
+      <c r="BM15" s="50"/>
+      <c r="BN15" s="50"/>
+      <c r="BO15" s="50"/>
+      <c r="BP15" s="50"/>
+      <c r="BQ15" s="50"/>
+      <c r="BR15" s="50"/>
+      <c r="BS15" s="50"/>
+      <c r="BT15" s="50"/>
+      <c r="BU15" s="50"/>
+      <c r="BV15" s="50"/>
+      <c r="BW15" s="50"/>
+      <c r="BX15" s="50"/>
+      <c r="BY15" s="50"/>
+      <c r="BZ15" s="50"/>
+      <c r="CA15" s="62"/>
+      <c r="CB15" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="2:80" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="70"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="14"/>
+      <c r="N16" s="14"/>
+      <c r="O16" s="14"/>
+      <c r="P16" s="15"/>
+      <c r="Q16" s="49"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="51"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="15"/>
+      <c r="Y16" s="71"/>
+      <c r="Z16" s="72"/>
+      <c r="AA16" s="73"/>
+      <c r="AB16" s="72"/>
+      <c r="AC16" s="72"/>
+      <c r="AD16" s="72"/>
+      <c r="AE16" s="72"/>
+      <c r="AF16" s="72"/>
+      <c r="AG16" s="72"/>
+      <c r="AH16" s="74"/>
+      <c r="AI16" s="71"/>
+      <c r="AJ16" s="72"/>
+      <c r="AK16" s="73"/>
+      <c r="AL16" s="72"/>
+      <c r="AM16" s="72"/>
+      <c r="AN16" s="72"/>
+      <c r="AO16" s="72"/>
+      <c r="AP16" s="72"/>
+      <c r="AQ16" s="72"/>
+      <c r="AR16" s="74"/>
+      <c r="AS16" s="75"/>
+      <c r="AT16" s="76"/>
+      <c r="AU16" s="77"/>
+      <c r="AV16" s="76"/>
+      <c r="AW16" s="76"/>
+      <c r="AX16" s="76"/>
+      <c r="AY16" s="76"/>
+      <c r="AZ16" s="76"/>
+      <c r="BA16" s="76"/>
+      <c r="BB16" s="78"/>
+      <c r="BC16" s="61"/>
+      <c r="BD16" s="50"/>
+      <c r="BE16" s="50"/>
+      <c r="BF16" s="50"/>
+      <c r="BG16" s="50"/>
+      <c r="BH16" s="50"/>
+      <c r="BI16" s="50"/>
+      <c r="BJ16" s="50"/>
+      <c r="BK16" s="50"/>
+      <c r="BL16" s="50"/>
+      <c r="BM16" s="50"/>
+      <c r="BN16" s="50"/>
+      <c r="BO16" s="50"/>
+      <c r="BP16" s="50"/>
+      <c r="BQ16" s="50"/>
+      <c r="BR16" s="50"/>
+      <c r="BS16" s="50"/>
+      <c r="BT16" s="50"/>
+      <c r="BU16" s="50"/>
+      <c r="BV16" s="50"/>
+      <c r="BW16" s="50"/>
+      <c r="BX16" s="50"/>
+      <c r="BY16" s="50"/>
+      <c r="BZ16" s="50"/>
+      <c r="CA16" s="62"/>
+      <c r="CB16" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="G17" s="79"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+      <c r="L17" s="80"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="80"/>
+      <c r="P17" s="81"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="82"/>
+      <c r="U17" s="82"/>
+      <c r="V17" s="82"/>
+      <c r="W17" s="82"/>
+      <c r="X17" s="82"/>
+      <c r="Y17" s="82"/>
+      <c r="Z17" s="82"/>
+      <c r="AA17" s="82"/>
+      <c r="AB17" s="82"/>
+      <c r="AC17" s="82"/>
+      <c r="AD17" s="82"/>
+      <c r="AE17" s="82"/>
+      <c r="AF17" s="82"/>
+      <c r="AG17" s="82"/>
+      <c r="AH17" s="82"/>
+      <c r="AI17" s="50"/>
+      <c r="AJ17" s="50"/>
+      <c r="AK17" s="82"/>
+      <c r="AL17" s="50"/>
+      <c r="AM17" s="50"/>
+      <c r="AN17" s="50"/>
+      <c r="AO17" s="50"/>
+      <c r="AP17" s="50"/>
+      <c r="AQ17" s="50"/>
+      <c r="AR17" s="50"/>
+      <c r="AS17" s="50"/>
+      <c r="AT17" s="50"/>
+      <c r="AU17" s="82"/>
+      <c r="AV17" s="50"/>
+      <c r="AW17" s="50"/>
+      <c r="AX17" s="50"/>
+      <c r="AY17" s="50"/>
+      <c r="AZ17" s="50"/>
+      <c r="BA17" s="50"/>
+      <c r="BB17" s="38"/>
+      <c r="BC17" s="49"/>
+      <c r="BD17" s="50"/>
+      <c r="BE17" s="50"/>
+      <c r="BF17" s="50"/>
+      <c r="BG17" s="50"/>
+      <c r="BH17" s="50"/>
+      <c r="BI17" s="50"/>
+      <c r="BJ17" s="50"/>
+      <c r="BK17" s="50"/>
+      <c r="BL17" s="50"/>
+      <c r="BM17" s="50"/>
+      <c r="BN17" s="50"/>
+      <c r="BO17" s="50"/>
+      <c r="BP17" s="50"/>
+      <c r="BQ17" s="50"/>
+      <c r="BR17" s="50"/>
+      <c r="BS17" s="50"/>
+      <c r="BT17" s="50"/>
+      <c r="BU17" s="50"/>
+      <c r="BV17" s="50"/>
+      <c r="BW17" s="50"/>
+      <c r="BX17" s="50"/>
+      <c r="BY17" s="50"/>
+      <c r="BZ17" s="50"/>
+      <c r="CA17" s="62"/>
+      <c r="CB17" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="G18" s="83"/>
+      <c r="H18" s="84"/>
+      <c r="I18" s="84"/>
+      <c r="J18" s="84"/>
+      <c r="K18" s="84"/>
+      <c r="L18" s="84"/>
+      <c r="M18" s="84"/>
+      <c r="N18" s="84"/>
+      <c r="O18" s="84"/>
+      <c r="P18" s="85"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="50"/>
+      <c r="W18" s="50"/>
+      <c r="X18" s="50"/>
+      <c r="Y18" s="50"/>
+      <c r="Z18" s="50"/>
+      <c r="AA18" s="50"/>
+      <c r="AB18" s="50"/>
+      <c r="AC18" s="50"/>
+      <c r="AD18" s="50"/>
+      <c r="AE18" s="50"/>
+      <c r="AF18" s="50"/>
+      <c r="AG18" s="50"/>
+      <c r="AH18" s="50"/>
+      <c r="AI18" s="50"/>
+      <c r="AJ18" s="50"/>
+      <c r="AK18" s="50"/>
+      <c r="AL18" s="50"/>
+      <c r="AM18" s="50"/>
+      <c r="AN18" s="50"/>
+      <c r="AO18" s="50"/>
+      <c r="AP18" s="50"/>
+      <c r="AQ18" s="50"/>
+      <c r="AR18" s="50"/>
+      <c r="AS18" s="50"/>
+      <c r="AT18" s="50"/>
+      <c r="AU18" s="50"/>
+      <c r="AV18" s="50"/>
+      <c r="AW18" s="50"/>
+      <c r="AX18" s="50"/>
+      <c r="AY18" s="50"/>
+      <c r="AZ18" s="50"/>
+      <c r="BA18" s="50"/>
+      <c r="BB18" s="50"/>
+      <c r="BC18" s="49"/>
+      <c r="BD18" s="50"/>
+      <c r="BE18" s="50"/>
+      <c r="BF18" s="50"/>
+      <c r="BG18" s="50"/>
+      <c r="BH18" s="50"/>
+      <c r="BI18" s="50"/>
+      <c r="BJ18" s="50"/>
+      <c r="BK18" s="50"/>
+      <c r="BL18" s="50"/>
+      <c r="BM18" s="50"/>
+      <c r="BN18" s="50"/>
+      <c r="BO18" s="50"/>
+      <c r="BP18" s="50"/>
+      <c r="BQ18" s="50"/>
+      <c r="BR18" s="50"/>
+      <c r="BS18" s="50"/>
+      <c r="BT18" s="50"/>
+      <c r="BU18" s="50"/>
+      <c r="BV18" s="50"/>
+      <c r="BW18" s="50"/>
+      <c r="BX18" s="50"/>
+      <c r="BY18" s="50"/>
+      <c r="BZ18" s="50"/>
+      <c r="CA18" s="62"/>
+      <c r="CB18" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="G19" s="83"/>
+      <c r="H19" s="84"/>
+      <c r="I19" s="84"/>
+      <c r="J19" s="84"/>
+      <c r="K19" s="84" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="84"/>
+      <c r="M19" s="84"/>
+      <c r="N19" s="84"/>
+      <c r="O19" s="84"/>
+      <c r="P19" s="86"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="50"/>
+      <c r="W19" s="50"/>
+      <c r="X19" s="50"/>
+      <c r="Y19" s="50"/>
+      <c r="Z19" s="50"/>
+      <c r="AA19" s="50"/>
+      <c r="AB19" s="50"/>
+      <c r="AC19" s="50"/>
+      <c r="AD19" s="50"/>
+      <c r="AE19" s="50"/>
+      <c r="AF19" s="50"/>
+      <c r="AG19" s="50"/>
+      <c r="AH19" s="50"/>
+      <c r="AI19" s="50"/>
+      <c r="AJ19" s="50"/>
+      <c r="AK19" s="50"/>
+      <c r="AL19" s="50"/>
+      <c r="AM19" s="50"/>
+      <c r="AN19" s="50"/>
+      <c r="AO19" s="50"/>
+      <c r="AP19" s="50"/>
+      <c r="AQ19" s="50"/>
+      <c r="AR19" s="50"/>
+      <c r="AS19" s="50"/>
+      <c r="AT19" s="50"/>
+      <c r="AU19" s="50"/>
+      <c r="AV19" s="50"/>
+      <c r="AW19" s="50"/>
+      <c r="AX19" s="50"/>
+      <c r="AY19" s="50"/>
+      <c r="AZ19" s="50"/>
+      <c r="BA19" s="50"/>
+      <c r="BB19" s="50"/>
+      <c r="BC19" s="49"/>
+      <c r="BD19" s="50"/>
+      <c r="BE19" s="50"/>
+      <c r="BF19" s="50"/>
+      <c r="BG19" s="50"/>
+      <c r="BH19" s="50"/>
+      <c r="BI19" s="50"/>
+      <c r="BJ19" s="50"/>
+      <c r="BK19" s="50"/>
+      <c r="BL19" s="50"/>
+      <c r="BM19" s="50"/>
+      <c r="BN19" s="50"/>
+      <c r="BO19" s="50"/>
+      <c r="BP19" s="50"/>
+      <c r="BQ19" s="50"/>
+      <c r="BR19" s="50"/>
+      <c r="BS19" s="50"/>
+      <c r="BT19" s="50"/>
+      <c r="BU19" s="50"/>
+      <c r="BV19" s="50"/>
+      <c r="BW19" s="50"/>
+      <c r="BX19" s="50"/>
+      <c r="BY19" s="50"/>
+      <c r="BZ19" s="50"/>
+      <c r="CA19" s="62"/>
+      <c r="CB19" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="G20" s="83"/>
+      <c r="H20" s="84"/>
+      <c r="I20" s="84"/>
+      <c r="J20" s="84"/>
+      <c r="K20" s="84"/>
+      <c r="L20" s="84"/>
+      <c r="M20" s="84"/>
+      <c r="N20" s="84"/>
+      <c r="O20" s="84"/>
+      <c r="P20" s="85"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="50"/>
+      <c r="W20" s="50"/>
+      <c r="X20" s="50"/>
+      <c r="Y20" s="50"/>
+      <c r="Z20" s="50"/>
+      <c r="AA20" s="50"/>
+      <c r="AB20" s="50"/>
+      <c r="AC20" s="50"/>
+      <c r="AD20" s="50"/>
+      <c r="AE20" s="50"/>
+      <c r="AF20" s="50"/>
+      <c r="AG20" s="50"/>
+      <c r="AH20" s="50"/>
+      <c r="AI20" s="50"/>
+      <c r="AJ20" s="50"/>
+      <c r="AK20" s="50"/>
+      <c r="AL20" s="50"/>
+      <c r="AM20" s="50"/>
+      <c r="AN20" s="50"/>
+      <c r="AO20" s="50"/>
+      <c r="AP20" s="50"/>
+      <c r="AQ20" s="50"/>
+      <c r="AR20" s="50"/>
+      <c r="AS20" s="50"/>
+      <c r="AT20" s="50"/>
+      <c r="AU20" s="50"/>
+      <c r="AV20" s="50"/>
+      <c r="AW20" s="50"/>
+      <c r="AX20" s="50"/>
+      <c r="AY20" s="50"/>
+      <c r="AZ20" s="50"/>
+      <c r="BA20" s="50"/>
+      <c r="BB20" s="50"/>
+      <c r="BC20" s="49"/>
+      <c r="BD20" s="50"/>
+      <c r="BE20" s="50"/>
+      <c r="BF20" s="50"/>
+      <c r="BG20" s="50"/>
+      <c r="BH20" s="50"/>
+      <c r="BI20" s="50"/>
+      <c r="BJ20" s="50"/>
+      <c r="BK20" s="50"/>
+      <c r="BL20" s="50"/>
+      <c r="BM20" s="50"/>
+      <c r="BN20" s="50"/>
+      <c r="BO20" s="50"/>
+      <c r="BP20" s="50"/>
+      <c r="BQ20" s="50"/>
+      <c r="BR20" s="50"/>
+      <c r="BS20" s="50"/>
+      <c r="BT20" s="50"/>
+      <c r="BU20" s="50"/>
+      <c r="BV20" s="50"/>
+      <c r="BW20" s="50"/>
+      <c r="BX20" s="50"/>
+      <c r="BY20" s="50"/>
+      <c r="BZ20" s="50"/>
+      <c r="CA20" s="62"/>
+      <c r="CB20" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:80" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="88"/>
+      <c r="I21" s="88"/>
+      <c r="J21" s="88"/>
+      <c r="K21" s="88"/>
+      <c r="L21" s="88"/>
+      <c r="M21" s="88"/>
+      <c r="N21" s="88"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="89"/>
+      <c r="Q21" s="90"/>
+      <c r="R21" s="90"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="90"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="50"/>
+      <c r="W21" s="50"/>
+      <c r="X21" s="50"/>
+      <c r="Y21" s="50"/>
+      <c r="Z21" s="50"/>
+      <c r="AA21" s="90"/>
+      <c r="AB21" s="50"/>
+      <c r="AC21" s="50"/>
+      <c r="AD21" s="50"/>
+      <c r="AE21" s="50"/>
+      <c r="AF21" s="50"/>
+      <c r="AG21" s="50"/>
+      <c r="AH21" s="50"/>
+      <c r="AI21" s="50"/>
+      <c r="AJ21" s="50"/>
+      <c r="AK21" s="90"/>
+      <c r="AL21" s="50"/>
+      <c r="AM21" s="50"/>
+      <c r="AN21" s="50"/>
+      <c r="AO21" s="50"/>
+      <c r="AP21" s="50"/>
+      <c r="AQ21" s="50"/>
+      <c r="AR21" s="50"/>
+      <c r="AS21" s="50"/>
+      <c r="AT21" s="50"/>
+      <c r="AU21" s="90"/>
+      <c r="AV21" s="50"/>
+      <c r="AW21" s="50"/>
+      <c r="AX21" s="50"/>
+      <c r="AY21" s="50"/>
+      <c r="AZ21" s="50"/>
+      <c r="BA21" s="50"/>
+      <c r="BB21" s="91"/>
+      <c r="BC21" s="49"/>
+      <c r="BD21" s="50"/>
+      <c r="BE21" s="50"/>
+      <c r="BF21" s="50"/>
+      <c r="BG21" s="50"/>
+      <c r="BH21" s="50"/>
+      <c r="BI21" s="50"/>
+      <c r="BJ21" s="50"/>
+      <c r="BK21" s="50"/>
+      <c r="BL21" s="50"/>
+      <c r="BM21" s="50"/>
+      <c r="BN21" s="50"/>
+      <c r="BO21" s="50"/>
+      <c r="BP21" s="50"/>
+      <c r="BQ21" s="50"/>
+      <c r="BR21" s="50"/>
+      <c r="BS21" s="50"/>
+      <c r="BT21" s="50"/>
+      <c r="BU21" s="50"/>
+      <c r="BV21" s="50"/>
+      <c r="BW21" s="50"/>
+      <c r="BX21" s="50"/>
+      <c r="BY21" s="50"/>
+      <c r="BZ21" s="50"/>
+      <c r="CA21" s="62"/>
+      <c r="CB21" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="19"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="17"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="18"/>
+      <c r="Y22" s="40"/>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="73"/>
+      <c r="AB22" s="41"/>
+      <c r="AC22" s="41"/>
+      <c r="AD22" s="41"/>
+      <c r="AE22" s="41"/>
+      <c r="AF22" s="41"/>
+      <c r="AG22" s="41"/>
+      <c r="AH22" s="42"/>
+      <c r="AI22" s="40"/>
+      <c r="AJ22" s="41"/>
+      <c r="AK22" s="73"/>
+      <c r="AL22" s="41"/>
+      <c r="AM22" s="41"/>
+      <c r="AN22" s="41"/>
+      <c r="AO22" s="41"/>
+      <c r="AP22" s="41"/>
+      <c r="AQ22" s="41"/>
+      <c r="AR22" s="42"/>
+      <c r="AS22" s="26"/>
+      <c r="AT22" s="27"/>
+      <c r="AU22" s="28"/>
+      <c r="AV22" s="27"/>
+      <c r="AW22" s="27"/>
+      <c r="AX22" s="27"/>
+      <c r="AY22" s="27"/>
+      <c r="AZ22" s="27"/>
+      <c r="BA22" s="27"/>
+      <c r="BB22" s="93"/>
+      <c r="BC22" s="61"/>
+      <c r="BD22" s="50"/>
+      <c r="BE22" s="50"/>
+      <c r="BF22" s="50"/>
+      <c r="BG22" s="50"/>
+      <c r="BH22" s="50"/>
+      <c r="BI22" s="50"/>
+      <c r="BJ22" s="50"/>
+      <c r="BK22" s="50"/>
+      <c r="BL22" s="50"/>
+      <c r="BM22" s="50"/>
+      <c r="BN22" s="50"/>
+      <c r="BO22" s="50"/>
+      <c r="BP22" s="50"/>
+      <c r="BQ22" s="50"/>
+      <c r="BR22" s="50"/>
+      <c r="BS22" s="50"/>
+      <c r="BT22" s="50"/>
+      <c r="BU22" s="50"/>
+      <c r="BV22" s="50"/>
+      <c r="BW22" s="50"/>
+      <c r="BX22" s="50"/>
+      <c r="BY22" s="50"/>
+      <c r="BZ22" s="50"/>
+      <c r="CA22" s="62"/>
+      <c r="CB22" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K23" s="20"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="20"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="21"/>
+      <c r="V23" s="21"/>
+      <c r="W23" s="21"/>
+      <c r="X23" s="21"/>
+      <c r="Y23" s="52"/>
+      <c r="Z23" s="53"/>
+      <c r="AA23" s="53"/>
+      <c r="AB23" s="53"/>
+      <c r="AC23" s="53"/>
+      <c r="AD23" s="53"/>
+      <c r="AE23" s="53"/>
+      <c r="AF23" s="53"/>
+      <c r="AG23" s="53"/>
+      <c r="AH23" s="54"/>
+      <c r="AI23" s="52"/>
+      <c r="AJ23" s="53"/>
+      <c r="AK23" s="53"/>
+      <c r="AL23" s="53"/>
+      <c r="AM23" s="53"/>
+      <c r="AN23" s="53"/>
+      <c r="AO23" s="53"/>
+      <c r="AP23" s="53"/>
+      <c r="AQ23" s="53"/>
+      <c r="AR23" s="54"/>
+      <c r="AS23" s="29"/>
+      <c r="AT23" s="30"/>
+      <c r="AU23" s="30"/>
+      <c r="AV23" s="30"/>
+      <c r="AW23" s="30"/>
+      <c r="AX23" s="30"/>
+      <c r="AY23" s="30"/>
+      <c r="AZ23" s="30"/>
+      <c r="BA23" s="30"/>
+      <c r="BB23" s="94"/>
+      <c r="BC23" s="61"/>
+      <c r="BD23" s="50"/>
+      <c r="BE23" s="50"/>
+      <c r="BF23" s="50"/>
+      <c r="BG23" s="50"/>
+      <c r="BH23" s="50"/>
+      <c r="BI23" s="50"/>
+      <c r="BJ23" s="50"/>
+      <c r="BK23" s="50"/>
+      <c r="BL23" s="50"/>
+      <c r="BM23" s="50"/>
+      <c r="BN23" s="50"/>
+      <c r="BO23" s="50"/>
+      <c r="BP23" s="50"/>
+      <c r="BQ23" s="50"/>
+      <c r="BR23" s="50"/>
+      <c r="BS23" s="50"/>
+      <c r="BT23" s="50"/>
+      <c r="BU23" s="50"/>
+      <c r="BV23" s="50"/>
+      <c r="BW23" s="50"/>
+      <c r="BX23" s="50"/>
+      <c r="BY23" s="50"/>
+      <c r="BZ23" s="50"/>
+      <c r="CA23" s="62"/>
+      <c r="CB23" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K24" s="20"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="92"/>
+      <c r="Q24" s="49"/>
+      <c r="R24" s="51"/>
+      <c r="S24" s="92"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="V24" s="21"/>
+      <c r="W24" s="21"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="52"/>
+      <c r="Z24" s="53"/>
+      <c r="AA24" s="53"/>
+      <c r="AB24" s="53"/>
+      <c r="AC24" s="53"/>
+      <c r="AD24" s="53"/>
+      <c r="AE24" s="53"/>
+      <c r="AF24" s="53"/>
+      <c r="AG24" s="53"/>
+      <c r="AH24" s="54"/>
+      <c r="AI24" s="52"/>
+      <c r="AJ24" s="53"/>
+      <c r="AK24" s="53"/>
+      <c r="AL24" s="53"/>
+      <c r="AM24" s="53"/>
+      <c r="AN24" s="53"/>
+      <c r="AO24" s="53"/>
+      <c r="AP24" s="53"/>
+      <c r="AQ24" s="53"/>
+      <c r="AR24" s="54"/>
+      <c r="AS24" s="29"/>
+      <c r="AT24" s="30"/>
+      <c r="AU24" s="30"/>
+      <c r="AV24" s="30"/>
+      <c r="AW24" s="30"/>
+      <c r="AX24" s="30"/>
+      <c r="AY24" s="30"/>
+      <c r="AZ24" s="30"/>
+      <c r="BA24" s="30"/>
+      <c r="BB24" s="94"/>
+      <c r="BC24" s="61"/>
+      <c r="BD24" s="50"/>
+      <c r="BE24" s="50"/>
+      <c r="BF24" s="50"/>
+      <c r="BG24" s="50"/>
+      <c r="BH24" s="50"/>
+      <c r="BI24" s="50"/>
+      <c r="BJ24" s="50"/>
+      <c r="BK24" s="50"/>
+      <c r="BL24" s="50"/>
+      <c r="BM24" s="50"/>
+      <c r="BN24" s="50"/>
+      <c r="BO24" s="50"/>
+      <c r="BP24" s="50"/>
+      <c r="BQ24" s="50"/>
+      <c r="BR24" s="50"/>
+      <c r="BS24" s="50"/>
+      <c r="BT24" s="50"/>
+      <c r="BU24" s="50"/>
+      <c r="BV24" s="50"/>
+      <c r="BW24" s="50"/>
+      <c r="BX24" s="50"/>
+      <c r="BY24" s="50"/>
+      <c r="BZ24" s="50"/>
+      <c r="CA24" s="62"/>
+      <c r="CB24" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K25" s="20"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="20"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="21"/>
+      <c r="V25" s="21"/>
+      <c r="W25" s="21"/>
+      <c r="X25" s="21"/>
+      <c r="Y25" s="52"/>
+      <c r="Z25" s="53"/>
+      <c r="AA25" s="53"/>
+      <c r="AB25" s="53"/>
+      <c r="AC25" s="53"/>
+      <c r="AD25" s="53"/>
+      <c r="AE25" s="53"/>
+      <c r="AF25" s="53"/>
+      <c r="AG25" s="53"/>
+      <c r="AH25" s="54"/>
+      <c r="AI25" s="52"/>
+      <c r="AJ25" s="53"/>
+      <c r="AK25" s="53"/>
+      <c r="AL25" s="53"/>
+      <c r="AM25" s="53"/>
+      <c r="AN25" s="53"/>
+      <c r="AO25" s="53"/>
+      <c r="AP25" s="53"/>
+      <c r="AQ25" s="53"/>
+      <c r="AR25" s="54"/>
+      <c r="AS25" s="29"/>
+      <c r="AT25" s="30"/>
+      <c r="AU25" s="30"/>
+      <c r="AV25" s="30"/>
+      <c r="AW25" s="30"/>
+      <c r="AX25" s="30"/>
+      <c r="AY25" s="30"/>
+      <c r="AZ25" s="30"/>
+      <c r="BA25" s="30"/>
+      <c r="BB25" s="94"/>
+      <c r="BC25" s="61"/>
+      <c r="BD25" s="50"/>
+      <c r="BE25" s="50"/>
+      <c r="BF25" s="50"/>
+      <c r="BG25" s="50"/>
+      <c r="BH25" s="50"/>
+      <c r="BI25" s="50"/>
+      <c r="BJ25" s="50"/>
+      <c r="BK25" s="50"/>
+      <c r="BL25" s="50"/>
+      <c r="BM25" s="50"/>
+      <c r="BN25" s="50"/>
+      <c r="BO25" s="50"/>
+      <c r="BP25" s="50"/>
+      <c r="BQ25" s="50"/>
+      <c r="BR25" s="50"/>
+      <c r="BS25" s="50"/>
+      <c r="BT25" s="50"/>
+      <c r="BU25" s="50"/>
+      <c r="BV25" s="50"/>
+      <c r="BW25" s="50"/>
+      <c r="BX25" s="50"/>
+      <c r="BY25" s="50"/>
+      <c r="BZ25" s="50"/>
+      <c r="CA25" s="62"/>
+      <c r="CB25" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:80" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="23"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="25"/>
+      <c r="Q26" s="96"/>
+      <c r="R26" s="97"/>
+      <c r="S26" s="23"/>
+      <c r="T26" s="24"/>
+      <c r="U26" s="24"/>
+      <c r="V26" s="24"/>
+      <c r="W26" s="24"/>
+      <c r="X26" s="24"/>
+      <c r="Y26" s="52"/>
+      <c r="Z26" s="53"/>
+      <c r="AA26" s="53"/>
+      <c r="AB26" s="53"/>
+      <c r="AC26" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD26" s="53"/>
+      <c r="AE26" s="53"/>
+      <c r="AF26" s="53"/>
+      <c r="AG26" s="53"/>
+      <c r="AH26" s="54"/>
+      <c r="AI26" s="52"/>
+      <c r="AJ26" s="53"/>
+      <c r="AK26" s="53"/>
+      <c r="AL26" s="53"/>
+      <c r="AM26" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="AN26" s="53"/>
+      <c r="AO26" s="53"/>
+      <c r="AP26" s="53"/>
+      <c r="AQ26" s="53"/>
+      <c r="AR26" s="54"/>
+      <c r="AS26" s="29"/>
+      <c r="AT26" s="30"/>
+      <c r="AU26" s="30"/>
+      <c r="AV26" s="30"/>
+      <c r="AW26" s="30"/>
+      <c r="AX26" s="30"/>
+      <c r="AY26" s="30"/>
+      <c r="AZ26" s="30"/>
+      <c r="BA26" s="30"/>
+      <c r="BB26" s="94"/>
+      <c r="BC26" s="61"/>
+      <c r="BD26" s="50"/>
+      <c r="BE26" s="50"/>
+      <c r="BF26" s="50"/>
+      <c r="BG26" s="50"/>
+      <c r="BH26" s="50"/>
+      <c r="BI26" s="50"/>
+      <c r="BJ26" s="50"/>
+      <c r="BK26" s="50"/>
+      <c r="BL26" s="50"/>
+      <c r="BM26" s="50"/>
+      <c r="BN26" s="50"/>
+      <c r="BO26" s="50"/>
+      <c r="BP26" s="50"/>
+      <c r="BQ26" s="50"/>
+      <c r="BR26" s="50"/>
+      <c r="BS26" s="50"/>
+      <c r="BT26" s="50"/>
+      <c r="BU26" s="50"/>
+      <c r="BV26" s="50"/>
+      <c r="BW26" s="50"/>
+      <c r="BX26" s="50"/>
+      <c r="BY26" s="50"/>
+      <c r="BZ26" s="50"/>
+      <c r="CA26" s="62"/>
+      <c r="CB26" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L27" s="5"/>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+      <c r="Y27" s="52"/>
+      <c r="Z27" s="53"/>
+      <c r="AA27" s="53"/>
+      <c r="AB27" s="53"/>
+      <c r="AC27" s="53"/>
+      <c r="AD27" s="53"/>
+      <c r="AE27" s="53"/>
+      <c r="AF27" s="53"/>
+      <c r="AG27" s="53"/>
+      <c r="AH27" s="54"/>
+      <c r="AI27" s="52"/>
+      <c r="AJ27" s="53"/>
+      <c r="AK27" s="53"/>
+      <c r="AL27" s="53"/>
+      <c r="AM27" s="53"/>
+      <c r="AN27" s="53"/>
+      <c r="AO27" s="53"/>
+      <c r="AP27" s="53"/>
+      <c r="AQ27" s="53"/>
+      <c r="AR27" s="54"/>
+      <c r="AS27" s="29"/>
+      <c r="AT27" s="30"/>
+      <c r="AU27" s="30"/>
+      <c r="AV27" s="30"/>
+      <c r="AW27" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="AX27" s="30"/>
+      <c r="AY27" s="30"/>
+      <c r="AZ27" s="30"/>
+      <c r="BA27" s="30"/>
+      <c r="BB27" s="94"/>
+      <c r="BC27" s="61"/>
+      <c r="BD27" s="50"/>
+      <c r="BE27" s="50"/>
+      <c r="BF27" s="50"/>
+      <c r="BG27" s="50"/>
+      <c r="BH27" s="50"/>
+      <c r="BI27" s="50"/>
+      <c r="BJ27" s="50"/>
+      <c r="BK27" s="50"/>
+      <c r="BL27" s="50"/>
+      <c r="BM27" s="50"/>
+      <c r="BN27" s="50"/>
+      <c r="BO27" s="50"/>
+      <c r="BP27" s="50"/>
+      <c r="BQ27" s="50"/>
+      <c r="BR27" s="50"/>
+      <c r="BS27" s="50"/>
+      <c r="BT27" s="50"/>
+      <c r="BU27" s="50"/>
+      <c r="BV27" s="50"/>
+      <c r="BW27" s="50"/>
+      <c r="BX27" s="50"/>
+      <c r="BY27" s="50"/>
+      <c r="BZ27" s="50"/>
+      <c r="CA27" s="62"/>
+      <c r="CB27" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y28" s="52"/>
+      <c r="Z28" s="53"/>
+      <c r="AA28" s="53"/>
+      <c r="AB28" s="53"/>
+      <c r="AC28" s="53"/>
+      <c r="AD28" s="53"/>
+      <c r="AE28" s="53"/>
+      <c r="AF28" s="53"/>
+      <c r="AG28" s="53"/>
+      <c r="AH28" s="54"/>
+      <c r="AI28" s="52"/>
+      <c r="AJ28" s="53"/>
+      <c r="AK28" s="53"/>
+      <c r="AL28" s="53"/>
+      <c r="AM28" s="53"/>
+      <c r="AN28" s="53"/>
+      <c r="AO28" s="53"/>
+      <c r="AP28" s="53"/>
+      <c r="AQ28" s="53"/>
+      <c r="AR28" s="54"/>
+      <c r="AS28" s="29"/>
+      <c r="AT28" s="30"/>
+      <c r="AU28" s="30"/>
+      <c r="AV28" s="30"/>
+      <c r="AW28" s="30"/>
+      <c r="AX28" s="30"/>
+      <c r="AY28" s="30"/>
+      <c r="AZ28" s="30"/>
+      <c r="BA28" s="30"/>
+      <c r="BB28" s="94"/>
+      <c r="BC28" s="61"/>
+      <c r="BD28" s="50"/>
+      <c r="BE28" s="50"/>
+      <c r="BF28" s="50"/>
+      <c r="BG28" s="50"/>
+      <c r="BH28" s="50"/>
+      <c r="BI28" s="50"/>
+      <c r="BJ28" s="50"/>
+      <c r="BK28" s="50"/>
+      <c r="BL28" s="50"/>
+      <c r="BM28" s="50"/>
+      <c r="BN28" s="50"/>
+      <c r="BO28" s="50"/>
+      <c r="BP28" s="50"/>
+      <c r="BQ28" s="50"/>
+      <c r="BR28" s="50"/>
+      <c r="BS28" s="50"/>
+      <c r="BT28" s="50"/>
+      <c r="BU28" s="50"/>
+      <c r="BV28" s="50"/>
+      <c r="BW28" s="50"/>
+      <c r="BX28" s="50"/>
+      <c r="BY28" s="50"/>
+      <c r="BZ28" s="50"/>
+      <c r="CA28" s="62"/>
+      <c r="CB28" s="1">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y29" s="52"/>
+      <c r="Z29" s="53"/>
+      <c r="AA29" s="53"/>
+      <c r="AB29" s="53"/>
+      <c r="AC29" s="53"/>
+      <c r="AD29" s="53"/>
+      <c r="AE29" s="53"/>
+      <c r="AF29" s="53"/>
+      <c r="AG29" s="53"/>
+      <c r="AH29" s="54"/>
+      <c r="AI29" s="52"/>
+      <c r="AJ29" s="53"/>
+      <c r="AK29" s="53"/>
+      <c r="AL29" s="53"/>
+      <c r="AM29" s="53"/>
+      <c r="AN29" s="53"/>
+      <c r="AO29" s="53"/>
+      <c r="AP29" s="53"/>
+      <c r="AQ29" s="53"/>
+      <c r="AR29" s="54"/>
+      <c r="AS29" s="29"/>
+      <c r="AT29" s="30"/>
+      <c r="AU29" s="30"/>
+      <c r="AV29" s="30"/>
+      <c r="AW29" s="30"/>
+      <c r="AX29" s="30"/>
+      <c r="AY29" s="30"/>
+      <c r="AZ29" s="30"/>
+      <c r="BA29" s="30"/>
+      <c r="BB29" s="94"/>
+      <c r="BC29" s="61"/>
+      <c r="BD29" s="50"/>
+      <c r="BE29" s="50"/>
+      <c r="BF29" s="50"/>
+      <c r="BG29" s="50"/>
+      <c r="BH29" s="50"/>
+      <c r="BI29" s="50"/>
+      <c r="BJ29" s="50"/>
+      <c r="BK29" s="50"/>
+      <c r="BL29" s="50"/>
+      <c r="BM29" s="50"/>
+      <c r="BN29" s="50"/>
+      <c r="BO29" s="50"/>
+      <c r="BP29" s="50"/>
+      <c r="BQ29" s="50"/>
+      <c r="BR29" s="50"/>
+      <c r="BS29" s="50"/>
+      <c r="BT29" s="50"/>
+      <c r="BU29" s="50"/>
+      <c r="BV29" s="50"/>
+      <c r="BW29" s="50"/>
+      <c r="BX29" s="50"/>
+      <c r="BY29" s="50"/>
+      <c r="BZ29" s="50"/>
+      <c r="CA29" s="62"/>
+      <c r="CB29" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y30" s="52"/>
+      <c r="Z30" s="53"/>
+      <c r="AA30" s="53"/>
+      <c r="AB30" s="53"/>
+      <c r="AC30" s="53"/>
+      <c r="AD30" s="53"/>
+      <c r="AE30" s="53"/>
+      <c r="AF30" s="53"/>
+      <c r="AG30" s="53"/>
+      <c r="AH30" s="54"/>
+      <c r="AI30" s="52"/>
+      <c r="AJ30" s="53"/>
+      <c r="AK30" s="53"/>
+      <c r="AL30" s="53"/>
+      <c r="AM30" s="53"/>
+      <c r="AN30" s="53"/>
+      <c r="AO30" s="53"/>
+      <c r="AP30" s="53"/>
+      <c r="AQ30" s="53"/>
+      <c r="AR30" s="54"/>
+      <c r="AS30" s="29"/>
+      <c r="AT30" s="30"/>
+      <c r="AU30" s="30"/>
+      <c r="AV30" s="30"/>
+      <c r="AW30" s="30"/>
+      <c r="AX30" s="30"/>
+      <c r="AY30" s="30"/>
+      <c r="AZ30" s="30"/>
+      <c r="BA30" s="30"/>
+      <c r="BB30" s="94"/>
+      <c r="BC30" s="61"/>
+      <c r="BD30" s="50"/>
+      <c r="BE30" s="50"/>
+      <c r="BF30" s="50"/>
+      <c r="BG30" s="50"/>
+      <c r="BH30" s="50"/>
+      <c r="BI30" s="50"/>
+      <c r="BJ30" s="50"/>
+      <c r="BK30" s="50"/>
+      <c r="BL30" s="50"/>
+      <c r="BM30" s="50"/>
+      <c r="BN30" s="50"/>
+      <c r="BO30" s="50"/>
+      <c r="BP30" s="50"/>
+      <c r="BQ30" s="50"/>
+      <c r="BR30" s="50"/>
+      <c r="BS30" s="50"/>
+      <c r="BT30" s="50"/>
+      <c r="BU30" s="50"/>
+      <c r="BV30" s="50"/>
+      <c r="BW30" s="50"/>
+      <c r="BX30" s="50"/>
+      <c r="BY30" s="50"/>
+      <c r="BZ30" s="50"/>
+      <c r="CA30" s="62"/>
+      <c r="CB30" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="31" spans="1:80" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Y31" s="71"/>
+      <c r="Z31" s="72"/>
+      <c r="AA31" s="72"/>
+      <c r="AB31" s="72"/>
+      <c r="AC31" s="72"/>
+      <c r="AD31" s="72"/>
+      <c r="AE31" s="72"/>
+      <c r="AF31" s="72"/>
+      <c r="AG31" s="72"/>
+      <c r="AH31" s="74"/>
+      <c r="AI31" s="71"/>
+      <c r="AJ31" s="72"/>
+      <c r="AK31" s="72"/>
+      <c r="AL31" s="72"/>
+      <c r="AM31" s="72"/>
+      <c r="AN31" s="72"/>
+      <c r="AO31" s="72"/>
+      <c r="AP31" s="72"/>
+      <c r="AQ31" s="72"/>
+      <c r="AR31" s="74"/>
+      <c r="AS31" s="31"/>
+      <c r="AT31" s="32"/>
+      <c r="AU31" s="32"/>
+      <c r="AV31" s="32"/>
+      <c r="AW31" s="32"/>
+      <c r="AX31" s="32"/>
+      <c r="AY31" s="32"/>
+      <c r="AZ31" s="32"/>
+      <c r="BA31" s="32"/>
+      <c r="BB31" s="95"/>
+      <c r="BC31" s="96"/>
+      <c r="BD31" s="91"/>
+      <c r="BE31" s="91"/>
+      <c r="BF31" s="91"/>
+      <c r="BG31" s="91"/>
+      <c r="BH31" s="91"/>
+      <c r="BI31" s="91"/>
+      <c r="BJ31" s="91"/>
+      <c r="BK31" s="91"/>
+      <c r="BL31" s="91"/>
+      <c r="BM31" s="91"/>
+      <c r="BN31" s="91"/>
+      <c r="BO31" s="91"/>
+      <c r="BP31" s="91"/>
+      <c r="BQ31" s="91"/>
+      <c r="BR31" s="91"/>
+      <c r="BS31" s="91"/>
+      <c r="BT31" s="91"/>
+      <c r="BU31" s="91"/>
+      <c r="BV31" s="91"/>
+      <c r="BW31" s="91"/>
+      <c r="BX31" s="91"/>
+      <c r="BY31" s="91"/>
+      <c r="BZ31" s="91"/>
+      <c r="CA31" s="97"/>
+      <c r="CB31" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="BC32" s="5"/>
+      <c r="BD32" s="5"/>
+      <c r="BE32" s="5"/>
+      <c r="BF32" s="5"/>
+      <c r="BG32" s="5"/>
+      <c r="BH32" s="5"/>
+      <c r="BI32" s="5"/>
+      <c r="BJ32" s="5"/>
+      <c r="BK32" s="5"/>
+      <c r="BL32" s="5"/>
+      <c r="BM32" s="5"/>
+      <c r="BN32" s="5"/>
+      <c r="BO32" s="5"/>
+      <c r="BP32" s="5"/>
+      <c r="BQ32" s="5"/>
+      <c r="BR32" s="5"/>
+      <c r="BS32" s="5"/>
+      <c r="BT32" s="5"/>
+      <c r="BU32" s="5"/>
+      <c r="BV32" s="5"/>
+      <c r="BW32" s="5"/>
+      <c r="BX32" s="5"/>
+      <c r="BY32" s="5"/>
+      <c r="BZ32" s="5"/>
+      <c r="CA32" s="5"/>
+    </row>
+    <row r="33" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BA8F45-DF05-4BC8-BB0A-EA311E0D4129}">
   <dimension ref="B2:F14"/>
   <sheetViews>
@@ -5978,7 +10491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="I1:CJ689"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added canteen prop base
</commit_message>
<xml_diff>
--- a/Assets/Documents/Game Document.xlsx
+++ b/Assets/Documents/Game Document.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\Horror_FPS\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF7BC00-9C71-403D-B39F-FC849F2C302E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF116B9-9F29-4A03-B7E5-2DF1C85399E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nursery_big" sheetId="6" r:id="rId1"/>
@@ -816,7 +816,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -826,14 +826,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1608,14 +1600,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6402,8 +6394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A7:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6568,7 +6560,7 @@
       <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="106" t="s">
+      <c r="C14" s="109" t="s">
         <v>5</v>
       </c>
       <c r="D14" s="33"/>
@@ -7065,7 +7057,7 @@
       <c r="C32" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="107" t="s">
+      <c r="H32" s="106" t="s">
         <v>39</v>
       </c>
       <c r="I32" s="34">
@@ -7091,7 +7083,7 @@
       <c r="D33" t="s">
         <v>44</v>
       </c>
-      <c r="H33" s="107" t="s">
+      <c r="H33" s="106" t="s">
         <v>40</v>
       </c>
       <c r="I33" s="34">
@@ -7409,7 +7401,7 @@
       <sortCondition ref="H17:H33"/>
     </sortState>
   </autoFilter>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -7429,119 +7421,119 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="107" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="107" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="4" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C4" s="108" t="s">
+      <c r="C4" s="107" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="5" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="109" t="s">
+      <c r="C5" s="108" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="6" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C6" s="108" t="s">
+      <c r="C6" s="107" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="7" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C7" s="108" t="s">
+      <c r="C7" s="107" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8" s="108" t="s">
+      <c r="C8" s="107" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="9" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="108" t="s">
+      <c r="C9" s="107" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="10" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="107" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="11" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C11" s="108" t="s">
+      <c r="C11" s="107" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="12" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C12" s="108" t="s">
+      <c r="C12" s="107" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="13" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="108" t="s">
+      <c r="C13" s="107" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14" s="108" t="s">
+      <c r="C14" s="107" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="15" spans="3:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="107" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16" s="108"/>
+      <c r="C16" s="107"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="108"/>
+      <c r="C17" s="107"/>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="108" t="s">
+      <c r="C18" s="107" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="108"/>
+      <c r="C19" s="107"/>
     </row>
     <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="108" t="s">
+      <c r="C20" s="107" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="108" t="s">
+      <c r="C21" s="107" t="s">
         <v>237</v>
       </c>
     </row>
     <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="108" t="s">
+      <c r="C22" s="107" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="108" t="s">
+      <c r="C23" s="107" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="108" t="s">
+      <c r="C24" s="107" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="108"/>
+      <c r="C25" s="107"/>
     </row>
     <row r="26" spans="3:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="C26" s="108" t="s">
+      <c r="C26" s="107" t="s">
         <v>240</v>
       </c>
     </row>
@@ -7555,7 +7547,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05D0279-7390-4F74-B85A-28B109ED7871}">
   <dimension ref="A1:CB689"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="X23" sqref="X23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added props and bug fixes
</commit_message>
<xml_diff>
--- a/Assets/Documents/Game Document.xlsx
+++ b/Assets/Documents/Game Document.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marco\Documents\GitHub\Horror_FPS\Assets\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF116B9-9F29-4A03-B7E5-2DF1C85399E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
   </bookViews>
   <sheets>
-    <sheet name="Nursery_big" sheetId="6" r:id="rId1"/>
-    <sheet name="Items" sheetId="5" r:id="rId2"/>
-    <sheet name="Gameplay flow description" sheetId="8" r:id="rId3"/>
-    <sheet name="Gameplay Flow" sheetId="9" r:id="rId4"/>
-    <sheet name="story" sheetId="7" r:id="rId5"/>
-    <sheet name="Floor Texture" sheetId="4" r:id="rId6"/>
+    <sheet name="Version" sheetId="10" r:id="rId1"/>
+    <sheet name="Nursery_big" sheetId="6" r:id="rId2"/>
+    <sheet name="Items" sheetId="5" r:id="rId3"/>
+    <sheet name="Gameplay flow description" sheetId="8" r:id="rId4"/>
+    <sheet name="Gameplay Flow" sheetId="9" r:id="rId5"/>
+    <sheet name="story" sheetId="7" r:id="rId6"/>
+    <sheet name="Floor Texture" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Items!$H$17:$K$33</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Items!$H$17:$K$33</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="268">
   <si>
     <t>Item</t>
   </si>
@@ -810,12 +810,39 @@
   </si>
   <si>
     <t>2 year olds' room</t>
+  </si>
+  <si>
+    <t>There is no standard, but you should do it in a way that makes sense to you and contains all the information you may need to track that build. I worked for a company that essentially broke it down like this:</t>
+  </si>
+  <si>
+    <t>[Major build number].[Minor build number].[Revision].[Package]</t>
+  </si>
+  <si>
+    <t>i.e. Version: 1.0.15.2</t>
+  </si>
+  <si>
+    <t>Major build number: This indicates a major milestone in the game, increment this when going from beta to release, from release to major updates.</t>
+  </si>
+  <si>
+    <t>Minor build number: Used for feature updates, large bug fixes etc.</t>
+  </si>
+  <si>
+    <t>Revision: Minor alterations on existing features, small bug fixes, etc.</t>
+  </si>
+  <si>
+    <t>Package: Your code stays the same, external library changes or asset file update.</t>
+  </si>
+  <si>
+    <t>Combined changes roll over to the most significant change. For example, if you're incrementing the minor build number, the revision and package both reset to 0.</t>
+  </si>
+  <si>
+    <t>Even though the categories are defined, there's still ambiguity for what kind of features actually cross over between a revision and a minor build number. It's up to you. If you make lists of the features that will need to be implemented before each increment, you'll also have a plan to follow, but in the end it's your decision as to what fits into each category.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1655,7 +1682,7 @@
         <xdr:cNvPr id="3" name="Conector: angular 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711DFAFC-B1D8-7E54-3150-058650349281}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{711DFAFC-B1D8-7E54-3150-058650349281}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1713,7 +1740,7 @@
         <xdr:cNvPr id="25" name="Conector recto 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F30FDA62-C088-1D01-BA26-3A3765AEF3ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F30FDA62-C088-1D01-BA26-3A3765AEF3ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1770,7 +1797,7 @@
         <xdr:cNvPr id="27" name="Conector recto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1A1767-EAE8-C126-F282-00C485F6BAE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CD1A1767-EAE8-C126-F282-00C485F6BAE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1827,7 +1854,7 @@
         <xdr:cNvPr id="29" name="Conector recto 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE75105F-5038-A32D-59C0-91BE1222DA69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE75105F-5038-A32D-59C0-91BE1222DA69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1882,7 +1909,7 @@
         <xdr:cNvPr id="36" name="Conector recto 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A174142-F93A-97F1-5D56-BC7B4820F608}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A174142-F93A-97F1-5D56-BC7B4820F608}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1937,7 +1964,7 @@
         <xdr:cNvPr id="38" name="Conector recto 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24C53F58-2C1C-BF7F-67A6-2F996551996F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24C53F58-2C1C-BF7F-67A6-2F996551996F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1992,7 +2019,7 @@
         <xdr:cNvPr id="40" name="Conector recto 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B563E933-3305-C976-D01A-6EFDB7D1FD70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B563E933-3305-C976-D01A-6EFDB7D1FD70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2047,7 +2074,7 @@
         <xdr:cNvPr id="46" name="Conector recto de flecha 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02C786B-2502-054E-EE28-3FA5C01C4114}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D02C786B-2502-054E-EE28-3FA5C01C4114}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2105,7 +2132,7 @@
         <xdr:cNvPr id="61" name="Conector: angular 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AA279DC-9447-1339-2D54-16662D29BA97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AA279DC-9447-1339-2D54-16662D29BA97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2165,7 +2192,7 @@
         <xdr:cNvPr id="69" name="Conector recto 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A89774-74F0-8E94-A964-218D87A0C69D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9A89774-74F0-8E94-A964-218D87A0C69D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2222,7 +2249,7 @@
         <xdr:cNvPr id="73" name="Conector recto de flecha 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33574CF7-C51D-0808-E350-CE01C347A03E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{33574CF7-C51D-0808-E350-CE01C347A03E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2278,7 +2305,7 @@
         <xdr:cNvPr id="78" name="Conector recto 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72837085-56AA-AD49-41F6-A3C55E63BFF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72837085-56AA-AD49-41F6-A3C55E63BFF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2335,7 +2362,7 @@
         <xdr:cNvPr id="80" name="Conector recto 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88603D43-5B4E-FB59-49C1-F6265EDA12B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88603D43-5B4E-FB59-49C1-F6265EDA12B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2392,7 +2419,7 @@
         <xdr:cNvPr id="86" name="Conector recto 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F84181-2698-0464-FEC8-D63C6321AACF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80F84181-2698-0464-FEC8-D63C6321AACF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2449,7 +2476,7 @@
         <xdr:cNvPr id="91" name="Conector recto de flecha 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9882E70A-D5E9-F0B1-2277-DC9793FD65E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9882E70A-D5E9-F0B1-2277-DC9793FD65E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2507,7 +2534,7 @@
         <xdr:cNvPr id="104" name="Conector: angular 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54AECD39-7FF0-D568-8DCD-04A7074BCD80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{54AECD39-7FF0-D568-8DCD-04A7074BCD80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2565,7 +2592,7 @@
         <xdr:cNvPr id="109" name="Conector recto 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296A9834-7F51-F21B-53E4-3B3B06E3A150}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{296A9834-7F51-F21B-53E4-3B3B06E3A150}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2620,7 +2647,7 @@
         <xdr:cNvPr id="114" name="Conector: angular 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F67CE7-F5C8-ACB0-C802-381702C6F4B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82F67CE7-F5C8-ACB0-C802-381702C6F4B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2677,7 +2704,7 @@
         <xdr:cNvPr id="117" name="Conector recto de flecha 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090E81F0-443E-6918-54B2-42919F5D96D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{090E81F0-443E-6918-54B2-42919F5D96D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2733,7 +2760,7 @@
         <xdr:cNvPr id="123" name="Conector recto 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577D3501-9328-F5EC-080B-DE787E7551BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{577D3501-9328-F5EC-080B-DE787E7551BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2790,7 +2817,7 @@
         <xdr:cNvPr id="125" name="Conector recto de flecha 124">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D5FEE7-92C5-D139-F653-230A3E01F91E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C0D5FEE7-92C5-D139-F653-230A3E01F91E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2848,7 +2875,7 @@
         <xdr:cNvPr id="127" name="Conector recto 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{850DE473-F646-5DB9-9469-7F1E8FCF7259}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{850DE473-F646-5DB9-9469-7F1E8FCF7259}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2905,7 +2932,7 @@
         <xdr:cNvPr id="132" name="Conector recto de flecha 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04063B44-D720-9CC2-C736-29613F51A4FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04063B44-D720-9CC2-C736-29613F51A4FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2961,7 +2988,7 @@
         <xdr:cNvPr id="140" name="Conector recto 139">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{361D4E4E-8242-6C2C-DFF9-19A39C9082E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{361D4E4E-8242-6C2C-DFF9-19A39C9082E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3018,7 +3045,7 @@
         <xdr:cNvPr id="142" name="Conector recto 141">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC83A31B-A200-55E0-3F0E-2341489ED50A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC83A31B-A200-55E0-3F0E-2341489ED50A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3075,7 +3102,7 @@
         <xdr:cNvPr id="144" name="Conector recto 143">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C65928E1-493D-61D1-DFAC-9CECAD98E827}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C65928E1-493D-61D1-DFAC-9CECAD98E827}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3132,7 +3159,7 @@
         <xdr:cNvPr id="146" name="Conector recto de flecha 145">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23DFFBB-6CFC-3A68-62EC-58AB42F1D419}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23DFFBB-6CFC-3A68-62EC-58AB42F1D419}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3190,7 +3217,7 @@
         <xdr:cNvPr id="155" name="Conector recto 154">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253621EA-18D1-B30C-8E68-1EC6806979FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{253621EA-18D1-B30C-8E68-1EC6806979FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3245,7 +3272,7 @@
         <xdr:cNvPr id="159" name="Conector recto de flecha 158">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A4666A-55E7-0490-41DF-625F9FDC464C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55A4666A-55E7-0490-41DF-625F9FDC464C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3301,7 +3328,7 @@
         <xdr:cNvPr id="161" name="Conector recto 160">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DE25EA7-44D2-25DB-74A3-14A3ADBEAE89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3DE25EA7-44D2-25DB-74A3-14A3ADBEAE89}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3603,7 +3630,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9E5FAB-1047-4072-92C4-3E2647FF44F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="127.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="107" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="107"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="107" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="107"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="107" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="107"/>
+    </row>
+    <row r="7" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="107" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="107" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="107" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="107" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="107"/>
+    </row>
+    <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="107" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="107"/>
+    </row>
+    <row r="14" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="107" t="s">
+        <v>267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="I1:CJ689"/>
   <sheetViews>
     <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
@@ -5727,674 +5835,675 @@
       <c r="CH32" s="5"/>
       <c r="CI32" s="5"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A7:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -7396,8 +7505,8 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="H17:K33" xr:uid="{00000000-0009-0000-0000-000003000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H18:K33">
+  <autoFilter ref="H17:K33">
+    <sortState ref="H18:K33">
       <sortCondition ref="H17:H33"/>
     </sortState>
   </autoFilter>
@@ -7407,8 +7516,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6CEA054-D4BB-43E1-86EC-CEF46B76B8DF}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="C2:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7543,8 +7653,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A05D0279-7390-4F74-B85A-28B109ED7871}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:CB689"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
@@ -10331,8 +10442,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BA8F45-DF05-4BC8-BB0A-EA311E0D4129}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="B2:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10475,8 +10587,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja7"/>
   <dimension ref="I1:CJ689"/>
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
@@ -12622,663 +12735,663 @@
       <c r="CH32" s="5"/>
       <c r="CI32" s="5"/>
     </row>
-    <row r="33" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Modified zombie in kitchen
</commit_message>
<xml_diff>
--- a/Assets/Documents/Game Document.xlsx
+++ b/Assets/Documents/Game Document.xlsx
@@ -1326,7 +1326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1652,6 +1652,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1699,7 +1705,7 @@
         <xdr:cNvPr id="3" name="Conector: angular 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{711DFAFC-B1D8-7E54-3150-058650349281}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{711DFAFC-B1D8-7E54-3150-058650349281}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1757,7 +1763,7 @@
         <xdr:cNvPr id="25" name="Conector recto 24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F30FDA62-C088-1D01-BA26-3A3765AEF3ED}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F30FDA62-C088-1D01-BA26-3A3765AEF3ED}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1814,7 +1820,7 @@
         <xdr:cNvPr id="27" name="Conector recto 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD1A1767-EAE8-C126-F282-00C485F6BAE7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CD1A1767-EAE8-C126-F282-00C485F6BAE7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1871,7 +1877,7 @@
         <xdr:cNvPr id="29" name="Conector recto 28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE75105F-5038-A32D-59C0-91BE1222DA69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE75105F-5038-A32D-59C0-91BE1222DA69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1926,7 +1932,7 @@
         <xdr:cNvPr id="36" name="Conector recto 35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A174142-F93A-97F1-5D56-BC7B4820F608}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A174142-F93A-97F1-5D56-BC7B4820F608}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1981,7 +1987,7 @@
         <xdr:cNvPr id="38" name="Conector recto 37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24C53F58-2C1C-BF7F-67A6-2F996551996F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24C53F58-2C1C-BF7F-67A6-2F996551996F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2036,7 +2042,7 @@
         <xdr:cNvPr id="40" name="Conector recto 39">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B563E933-3305-C976-D01A-6EFDB7D1FD70}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B563E933-3305-C976-D01A-6EFDB7D1FD70}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2091,7 +2097,7 @@
         <xdr:cNvPr id="46" name="Conector recto de flecha 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D02C786B-2502-054E-EE28-3FA5C01C4114}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D02C786B-2502-054E-EE28-3FA5C01C4114}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2149,7 +2155,7 @@
         <xdr:cNvPr id="61" name="Conector: angular 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AA279DC-9447-1339-2D54-16662D29BA97}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AA279DC-9447-1339-2D54-16662D29BA97}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2209,7 +2215,7 @@
         <xdr:cNvPr id="69" name="Conector recto 68">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9A89774-74F0-8E94-A964-218D87A0C69D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9A89774-74F0-8E94-A964-218D87A0C69D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2266,7 +2272,7 @@
         <xdr:cNvPr id="73" name="Conector recto de flecha 72">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33574CF7-C51D-0808-E350-CE01C347A03E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{33574CF7-C51D-0808-E350-CE01C347A03E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2322,7 +2328,7 @@
         <xdr:cNvPr id="78" name="Conector recto 77">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72837085-56AA-AD49-41F6-A3C55E63BFF8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72837085-56AA-AD49-41F6-A3C55E63BFF8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2379,7 +2385,7 @@
         <xdr:cNvPr id="80" name="Conector recto 79">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88603D43-5B4E-FB59-49C1-F6265EDA12B0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88603D43-5B4E-FB59-49C1-F6265EDA12B0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2436,7 +2442,7 @@
         <xdr:cNvPr id="86" name="Conector recto 85">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80F84181-2698-0464-FEC8-D63C6321AACF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80F84181-2698-0464-FEC8-D63C6321AACF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2493,7 +2499,7 @@
         <xdr:cNvPr id="91" name="Conector recto de flecha 90">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9882E70A-D5E9-F0B1-2277-DC9793FD65E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9882E70A-D5E9-F0B1-2277-DC9793FD65E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2551,7 +2557,7 @@
         <xdr:cNvPr id="104" name="Conector: angular 103">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54AECD39-7FF0-D568-8DCD-04A7074BCD80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{54AECD39-7FF0-D568-8DCD-04A7074BCD80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2609,7 +2615,7 @@
         <xdr:cNvPr id="109" name="Conector recto 108">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{296A9834-7F51-F21B-53E4-3B3B06E3A150}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{296A9834-7F51-F21B-53E4-3B3B06E3A150}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2664,7 +2670,7 @@
         <xdr:cNvPr id="114" name="Conector: angular 113">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82F67CE7-F5C8-ACB0-C802-381702C6F4B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82F67CE7-F5C8-ACB0-C802-381702C6F4B2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2721,7 +2727,7 @@
         <xdr:cNvPr id="117" name="Conector recto de flecha 116">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{090E81F0-443E-6918-54B2-42919F5D96D8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{090E81F0-443E-6918-54B2-42919F5D96D8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2777,7 +2783,7 @@
         <xdr:cNvPr id="123" name="Conector recto 122">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{577D3501-9328-F5EC-080B-DE787E7551BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{577D3501-9328-F5EC-080B-DE787E7551BA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2834,7 +2840,7 @@
         <xdr:cNvPr id="125" name="Conector recto de flecha 124">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0D5FEE7-92C5-D139-F653-230A3E01F91E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C0D5FEE7-92C5-D139-F653-230A3E01F91E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2892,7 +2898,7 @@
         <xdr:cNvPr id="127" name="Conector recto 126">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{850DE473-F646-5DB9-9469-7F1E8FCF7259}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{850DE473-F646-5DB9-9469-7F1E8FCF7259}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2949,7 +2955,7 @@
         <xdr:cNvPr id="132" name="Conector recto de flecha 131">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04063B44-D720-9CC2-C736-29613F51A4FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04063B44-D720-9CC2-C736-29613F51A4FD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3005,7 +3011,7 @@
         <xdr:cNvPr id="140" name="Conector recto 139">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{361D4E4E-8242-6C2C-DFF9-19A39C9082E4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{361D4E4E-8242-6C2C-DFF9-19A39C9082E4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3062,7 +3068,7 @@
         <xdr:cNvPr id="142" name="Conector recto 141">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC83A31B-A200-55E0-3F0E-2341489ED50A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC83A31B-A200-55E0-3F0E-2341489ED50A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3119,7 +3125,7 @@
         <xdr:cNvPr id="144" name="Conector recto 143">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C65928E1-493D-61D1-DFAC-9CECAD98E827}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C65928E1-493D-61D1-DFAC-9CECAD98E827}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3176,7 +3182,7 @@
         <xdr:cNvPr id="146" name="Conector recto de flecha 145">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E23DFFBB-6CFC-3A68-62EC-58AB42F1D419}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23DFFBB-6CFC-3A68-62EC-58AB42F1D419}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3234,7 +3240,7 @@
         <xdr:cNvPr id="155" name="Conector recto 154">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253621EA-18D1-B30C-8E68-1EC6806979FA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{253621EA-18D1-B30C-8E68-1EC6806979FA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3289,7 +3295,7 @@
         <xdr:cNvPr id="159" name="Conector recto de flecha 158">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{55A4666A-55E7-0490-41DF-625F9FDC464C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55A4666A-55E7-0490-41DF-625F9FDC464C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3345,7 +3351,7 @@
         <xdr:cNvPr id="161" name="Conector recto 160">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DE25EA7-44D2-25DB-74A3-14A3ADBEAE89}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3DE25EA7-44D2-25DB-74A3-14A3ADBEAE89}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -10609,8 +10615,8 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="I1:CN687"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="CI29" sqref="T7:CI29"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6:CI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10625,209 +10631,206 @@
     <row r="4" spans="10:92" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="10:92" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="10:92" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="T6" s="1">
+      <c r="U6" s="1">
         <v>1</v>
       </c>
-      <c r="U6" s="1">
+      <c r="V6" s="1">
         <v>2</v>
       </c>
-      <c r="V6" s="1">
+      <c r="W6" s="1">
         <v>3</v>
       </c>
-      <c r="W6" s="1">
+      <c r="X6" s="1">
         <v>4</v>
       </c>
-      <c r="X6" s="1">
+      <c r="Y6" s="1">
         <v>5</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Z6" s="3">
         <v>6</v>
       </c>
-      <c r="Z6" s="3">
+      <c r="AA6" s="3">
         <v>7</v>
       </c>
-      <c r="AA6" s="3">
+      <c r="AB6" s="3">
         <v>8</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AC6" s="3">
         <v>9</v>
       </c>
-      <c r="AC6" s="3">
+      <c r="AD6" s="3">
         <v>10</v>
       </c>
-      <c r="AD6" s="3">
+      <c r="AE6" s="3">
         <v>11</v>
       </c>
-      <c r="AE6" s="3">
+      <c r="AF6" s="3">
         <v>12</v>
       </c>
-      <c r="AF6" s="3">
+      <c r="AG6" s="3">
         <v>13</v>
       </c>
-      <c r="AG6" s="3">
+      <c r="AH6" s="3">
         <v>14</v>
       </c>
-      <c r="AH6" s="3">
+      <c r="AI6" s="3">
         <v>15</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="AJ6" s="3">
         <v>16</v>
       </c>
-      <c r="AJ6" s="3">
+      <c r="AK6" s="3">
         <v>17</v>
       </c>
-      <c r="AK6" s="3">
+      <c r="AL6" s="3">
         <v>18</v>
       </c>
-      <c r="AL6" s="3">
+      <c r="AM6" s="3">
         <v>19</v>
       </c>
-      <c r="AM6" s="3">
+      <c r="AN6" s="3">
         <v>20</v>
       </c>
-      <c r="AN6" s="3">
+      <c r="AO6" s="3">
         <v>21</v>
       </c>
-      <c r="AO6" s="3">
+      <c r="AP6" s="3">
         <v>22</v>
       </c>
-      <c r="AP6" s="3">
+      <c r="AQ6" s="3">
         <v>23</v>
       </c>
-      <c r="AQ6" s="3">
+      <c r="AR6" s="3">
         <v>24</v>
       </c>
-      <c r="AR6" s="3">
+      <c r="AS6" s="3">
         <v>25</v>
       </c>
-      <c r="AS6" s="3">
+      <c r="AT6" s="3">
         <v>26</v>
       </c>
-      <c r="AT6" s="3">
+      <c r="AU6" s="3">
         <v>27</v>
       </c>
-      <c r="AU6" s="3">
+      <c r="AV6" s="3">
         <v>28</v>
       </c>
-      <c r="AV6" s="3">
+      <c r="AW6" s="3">
         <v>29</v>
       </c>
-      <c r="AW6" s="3">
+      <c r="AX6" s="3">
         <v>30</v>
       </c>
-      <c r="AX6" s="3">
+      <c r="AY6" s="3">
         <v>31</v>
       </c>
-      <c r="AY6" s="3">
+      <c r="AZ6" s="3">
         <v>32</v>
       </c>
-      <c r="AZ6" s="3">
+      <c r="BA6" s="3">
         <v>33</v>
       </c>
-      <c r="BA6" s="3">
+      <c r="BB6" s="3">
         <v>34</v>
       </c>
-      <c r="BB6" s="3">
+      <c r="BC6" s="3">
         <v>35</v>
       </c>
-      <c r="BC6" s="3">
+      <c r="BD6" s="3">
         <v>36</v>
       </c>
-      <c r="BD6" s="3">
+      <c r="BE6" s="3">
         <v>37</v>
       </c>
-      <c r="BE6" s="3">
+      <c r="BF6" s="3">
         <v>38</v>
       </c>
-      <c r="BF6" s="3">
+      <c r="BG6" s="3">
         <v>39</v>
       </c>
-      <c r="BG6" s="3">
+      <c r="BH6" s="3">
         <v>40</v>
       </c>
-      <c r="BH6" s="3">
+      <c r="BI6" s="3">
         <v>41</v>
       </c>
-      <c r="BI6" s="3">
+      <c r="BJ6" s="3">
         <v>42</v>
       </c>
-      <c r="BJ6" s="3">
+      <c r="BK6" s="3">
         <v>43</v>
       </c>
-      <c r="BK6" s="3">
+      <c r="BL6" s="3">
         <v>44</v>
       </c>
-      <c r="BL6" s="3">
+      <c r="BM6" s="3">
         <v>45</v>
       </c>
-      <c r="BM6" s="3">
+      <c r="BN6" s="3">
         <v>46</v>
       </c>
-      <c r="BN6" s="3">
+      <c r="BO6" s="3">
         <v>47</v>
       </c>
-      <c r="BO6" s="3">
+      <c r="BP6" s="3">
         <v>48</v>
       </c>
-      <c r="BP6" s="3">
+      <c r="BQ6" s="3">
         <v>49</v>
       </c>
-      <c r="BQ6" s="3">
+      <c r="BR6" s="3">
         <v>50</v>
       </c>
-      <c r="BR6" s="3">
+      <c r="BS6" s="3">
         <v>51</v>
       </c>
-      <c r="BS6" s="3">
+      <c r="BT6" s="3">
         <v>52</v>
       </c>
-      <c r="BT6" s="3">
+      <c r="BU6" s="3">
         <v>53</v>
       </c>
-      <c r="BU6" s="3">
+      <c r="BV6" s="3">
         <v>54</v>
       </c>
-      <c r="BV6" s="3">
+      <c r="BW6" s="3">
         <v>55</v>
       </c>
-      <c r="BW6" s="3">
+      <c r="BX6" s="3">
         <v>56</v>
       </c>
-      <c r="BX6" s="3">
+      <c r="BY6" s="3">
         <v>57</v>
       </c>
-      <c r="BY6" s="3">
+      <c r="BZ6" s="3">
         <v>58</v>
       </c>
-      <c r="BZ6" s="3">
+      <c r="CA6" s="3">
         <v>59</v>
       </c>
-      <c r="CA6" s="3">
+      <c r="CB6" s="3">
         <v>60</v>
       </c>
-      <c r="CB6" s="3">
+      <c r="CC6" s="3">
         <v>61</v>
       </c>
-      <c r="CC6" s="3">
+      <c r="CD6" s="3">
         <v>62</v>
       </c>
-      <c r="CD6" s="3">
+      <c r="CE6" s="3">
         <v>63</v>
       </c>
-      <c r="CE6" s="3">
+      <c r="CF6" s="3">
         <v>64</v>
       </c>
-      <c r="CF6" s="3">
+      <c r="CG6" s="3">
         <v>65</v>
       </c>
-      <c r="CG6" s="3">
+      <c r="CH6" s="3">
         <v>66</v>
       </c>
-      <c r="CH6" s="3">
+      <c r="CI6" s="3">
         <v>67</v>
-      </c>
-      <c r="CI6" s="3">
-        <v>68</v>
       </c>
       <c r="CJ6" s="3"/>
       <c r="CK6" s="3"/>
@@ -11821,9 +11824,8 @@
       <c r="Q20" s="5"/>
       <c r="R20" s="5"/>
       <c r="S20" s="6"/>
-      <c r="T20" s="99"/>
-      <c r="U20" s="99"/>
-      <c r="V20" s="99"/>
+      <c r="U20" s="113"/>
+      <c r="V20" s="113"/>
       <c r="W20" s="99"/>
       <c r="X20" s="99"/>
       <c r="Y20" s="99"/>
@@ -11895,9 +11897,8 @@
     </row>
     <row r="21" spans="9:88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S21" s="2"/>
-      <c r="T21" s="99"/>
-      <c r="U21" s="100"/>
-      <c r="V21" s="100"/>
+      <c r="U21" s="113"/>
+      <c r="V21" s="114"/>
       <c r="W21" s="100"/>
       <c r="X21" s="100"/>
       <c r="Y21" s="99"/>
@@ -11969,9 +11970,8 @@
     </row>
     <row r="22" spans="9:88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S22" s="2"/>
-      <c r="T22" s="99"/>
-      <c r="U22" s="100"/>
-      <c r="V22" s="100"/>
+      <c r="U22" s="113"/>
+      <c r="V22" s="114"/>
       <c r="W22" s="100"/>
       <c r="X22" s="100"/>
       <c r="Y22" s="99"/>
@@ -12043,9 +12043,8 @@
     </row>
     <row r="23" spans="9:88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S23" s="2"/>
-      <c r="T23" s="99"/>
-      <c r="U23" s="100"/>
-      <c r="V23" s="100"/>
+      <c r="U23" s="113"/>
+      <c r="V23" s="114"/>
       <c r="W23" s="100"/>
       <c r="X23" s="100"/>
       <c r="Y23" s="99"/>
@@ -12117,9 +12116,8 @@
     </row>
     <row r="24" spans="9:88" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="S24" s="2"/>
-      <c r="T24" s="99"/>
-      <c r="U24" s="99"/>
-      <c r="V24" s="99"/>
+      <c r="U24" s="113"/>
+      <c r="V24" s="113"/>
       <c r="W24" s="99"/>
       <c r="X24" s="99"/>
       <c r="Y24" s="99"/>

</xml_diff>

<commit_message>
Last demo version with first design
</commit_message>
<xml_diff>
--- a/Assets/Documents/Game Document.xlsx
+++ b/Assets/Documents/Game Document.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="10" r:id="rId1"/>
@@ -1685,1712 +1685,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>238125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>272142</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Conector: angular 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{711DFAFC-B1D8-7E54-3150-058650349281}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3876675" y="2524125"/>
-          <a:ext cx="1538967" cy="1353911"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 74138"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>160734</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>163286</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>160734</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="25" name="Conector recto 24">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F30FDA62-C088-1D01-BA26-3A3765AEF3ED}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="14733984" y="2449286"/>
-          <a:ext cx="2552" cy="1711948"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>136071</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>163286</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="27" name="Conector recto 26">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CD1A1767-EAE8-C126-F282-00C485F6BAE7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="13280571" y="4150179"/>
-          <a:ext cx="1455965" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>148828</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>149679</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>149679</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>196453</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="29" name="Conector recto 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AE75105F-5038-A32D-59C0-91BE1222DA69}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="13293328" y="4150179"/>
-          <a:ext cx="851" cy="1189774"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>184547</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>160734</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>204107</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="36" name="Conector recto 35">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A174142-F93A-97F1-5D56-BC7B4820F608}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5238750" y="5328047"/>
-          <a:ext cx="8066484" cy="19560"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>226219</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>107156</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>214312</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="38" name="Conector recto 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{24C53F58-2C1C-BF7F-67A6-2F996551996F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5238750" y="3940969"/>
-          <a:ext cx="11906" cy="1416843"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>231321</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>231321</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="40" name="Conector recto 39">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B563E933-3305-C976-D01A-6EFDB7D1FD70}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5238750" y="3946071"/>
-          <a:ext cx="830036" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>49</xdr:col>
-      <xdr:colOff>68036</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>51</xdr:col>
-      <xdr:colOff>176893</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>176893</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="46" name="Conector recto de flecha 45">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D02C786B-2502-054E-EE28-3FA5C01C4114}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="14069786" y="2462893"/>
-          <a:ext cx="680357" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>266704</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="61" name="Conector: angular 60">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AA279DC-9447-1339-2D54-16662D29BA97}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000" flipV="1">
-          <a:off x="4552954" y="5572125"/>
-          <a:ext cx="8839196" cy="1162050"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 98060"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>239184</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>266700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>239184</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="69" name="Conector recto 68">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C9A89774-74F0-8E94-A964-218D87A0C69D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="13383684" y="4552950"/>
-          <a:ext cx="0" cy="1028700"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="73" name="Conector recto de flecha 72">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{33574CF7-C51D-0808-E350-CE01C347A03E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4591050" y="6819900"/>
-          <a:ext cx="552450" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>59531</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>5953</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="78" name="Conector recto 77">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{72837085-56AA-AD49-41F6-A3C55E63BFF8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5000625" y="5715000"/>
-          <a:ext cx="8203406" cy="5953"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>276225</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="80" name="Conector recto 79">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88603D43-5B4E-FB59-49C1-F6265EDA12B0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5010150" y="5705475"/>
-          <a:ext cx="0" cy="962025"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="86" name="Conector recto 85">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{80F84181-2698-0464-FEC8-D63C6321AACF}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5010150" y="6667500"/>
-          <a:ext cx="133350" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>5953</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>5953</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="91" name="Conector recto de flecha 90">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9882E70A-D5E9-F0B1-2277-DC9793FD65E5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13192125" y="5720953"/>
-          <a:ext cx="0" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>142878</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>209551</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="104" name="Conector: angular 103">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{54AECD39-7FF0-D568-8DCD-04A7074BCD80}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="10800000">
-          <a:off x="4552950" y="3857628"/>
-          <a:ext cx="8743950" cy="1781173"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 96514"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>209550</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="109" name="Conector recto 108">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{296A9834-7F51-F21B-53E4-3B3B06E3A150}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13296900" y="5638800"/>
-          <a:ext cx="0" cy="361950"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>228600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>147205</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>60614</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="114" name="Conector: angular 113">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{82F67CE7-F5C8-ACB0-C802-381702C6F4B2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4581525" y="3943350"/>
-          <a:ext cx="2995180" cy="1546514"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 12128"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>121227</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>51955</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>138545</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>8659</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="117" name="Conector recto de flecha 116">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{090E81F0-443E-6918-54B2-42919F5D96D8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="7550727" y="5481205"/>
-          <a:ext cx="17318" cy="528204"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="123" name="Conector recto 122">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{577D3501-9328-F5EC-080B-DE787E7551BA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="7667625" y="5838825"/>
-          <a:ext cx="2714625" cy="9525"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>257175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="125" name="Conector recto de flecha 124">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C0D5FEE7-92C5-D139-F653-230A3E01F91E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10382250" y="4543425"/>
-          <a:ext cx="0" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>279400</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="127" name="Conector recto 126">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{850DE473-F646-5DB9-9469-7F1E8FCF7259}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7664450" y="5842000"/>
-          <a:ext cx="0" cy="152400"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>181841</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>8659</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>199159</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="132" name="Conector recto de flecha 131">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{04063B44-D720-9CC2-C736-29613F51A4FD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="10468841" y="4580659"/>
-          <a:ext cx="17318" cy="1420091"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>51955</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>60614</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="140" name="Conector recto 139">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{361D4E4E-8242-6C2C-DFF9-19A39C9082E4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="10338955" y="5143500"/>
-          <a:ext cx="8659" cy="857250"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>277091</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>60614</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>8659</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="142" name="Conector recto 141">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{BC83A31B-A200-55E0-3F0E-2341489ED50A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="5134841" y="5143500"/>
-          <a:ext cx="5212773" cy="8659"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>277091</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>277091</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>8659</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="144" name="Conector recto 143">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C65928E1-493D-61D1-DFAC-9CECAD98E827}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="5134841" y="2441864"/>
-          <a:ext cx="0" cy="2710295"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>277091</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>8659</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="146" name="Conector recto de flecha 145">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E23DFFBB-6CFC-3A68-62EC-58AB42F1D419}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5134841" y="2441864"/>
-          <a:ext cx="303068" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:lumMod val="75000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>138545</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>43295</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>138545</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="155" name="Conector recto 154">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{253621EA-18D1-B30C-8E68-1EC6806979FA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4710545" y="2329295"/>
-          <a:ext cx="0" cy="2970069"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>268432</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>147205</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>138545</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>155864</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="159" name="Conector recto de flecha 158">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{55A4666A-55E7-0490-41DF-625F9FDC464C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="4554682" y="5290705"/>
-          <a:ext cx="155863" cy="8659"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>129886</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>43295</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>51955</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="161" name="Conector recto 160">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{3DE25EA7-44D2-25DB-74A3-14A3ADBEAE89}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4701886" y="2329295"/>
-          <a:ext cx="727364" cy="8660"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="28575">
-          <a:solidFill>
-            <a:schemeClr val="accent2"/>
-          </a:solidFill>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent2"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent2"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7681,8 +5975,8 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:CB689"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X23" sqref="X23"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="BM11" sqref="BM11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10461,7 +8755,6 @@
     <row r="689" ht="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10615,7 +8908,7 @@
   <sheetPr codeName="Hoja7"/>
   <dimension ref="I1:CN687"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="L1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="U6" sqref="U6:CI6"/>
     </sheetView>
   </sheetViews>

</xml_diff>